<commit_message>
Binary Search Tree added
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="532">
   <si>
     <t xml:space="preserve">YES(Iterative &amp; recursive)</t>
   </si>
@@ -862,15 +862,24 @@
     <t xml:space="preserve">Fina a value in a BST</t>
   </si>
   <si>
+    <t xml:space="preserve">y(search and insert leaf)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Deletion of a node in a BST</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(recursive and iterative)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Find min and max value in a BST</t>
   </si>
   <si>
     <t xml:space="preserve">Find inorder successor and inorder predecessor in a BST</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(see condtion if key not present in tree)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Check if a tree is a BST or not </t>
   </si>
   <si>
@@ -883,6 +892,9 @@
     <t xml:space="preserve">Construct BST from preorder traversal</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(Check modified recursion (using range))</t>
+  </si>
+  <si>
     <t xml:space="preserve">Convert Binary tree into BST</t>
   </si>
   <si>
@@ -898,12 +910,18 @@
     <t xml:space="preserve">Find Kth smallest element in a BST</t>
   </si>
   <si>
+    <t xml:space="preserve">y(similar to previous)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Count pairs from 2 BST whose sum is equal to given value "X"</t>
   </si>
   <si>
     <t xml:space="preserve">Find the median of BST in O(n) time and O(1) space</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(MORRIS INORDER TRAVERSAL)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Count BST ndoes that lie in a given range</t>
   </si>
   <si>
@@ -920,6 +938,9 @@
   </si>
   <si>
     <t xml:space="preserve">Largest BST in a Binary Tree [ V.V.V.V.V IMP ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES(postorder return info of each subtree)</t>
   </si>
   <si>
     <t xml:space="preserve">Flatten BST to sorted list</t>
@@ -1908,15 +1929,16 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A190" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C212" activeCellId="0" sqref="C212"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A209" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C237" activeCellId="0" sqref="C237"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="111.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="44.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="4" style="0" width="11.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4166,7 +4188,7 @@
         <v>269</v>
       </c>
       <c r="C214" s="6" t="s">
-        <v>119</v>
+        <v>270</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4174,21 +4196,21 @@
         <v>268</v>
       </c>
       <c r="B215" s="8" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C215" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="216" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="7" t="s">
         <v>268</v>
       </c>
       <c r="B216" s="8" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C216" s="6" t="s">
-        <v>119</v>
+        <v>8</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4196,10 +4218,10 @@
         <v>268</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C217" s="6" t="s">
-        <v>119</v>
+        <v>275</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4207,10 +4229,10 @@
         <v>268</v>
       </c>
       <c r="B218" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="C218" s="6" t="s">
-        <v>119</v>
+        <v>276</v>
+      </c>
+      <c r="C218" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4218,10 +4240,10 @@
         <v>268</v>
       </c>
       <c r="B219" s="8" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C219" s="6" t="s">
-        <v>119</v>
+        <v>8</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4229,10 +4251,10 @@
         <v>268</v>
       </c>
       <c r="B220" s="12" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="C220" s="6" t="s">
-        <v>119</v>
+        <v>8</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4240,10 +4262,10 @@
         <v>268</v>
       </c>
       <c r="B221" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="C221" s="6" t="s">
-        <v>119</v>
+        <v>279</v>
+      </c>
+      <c r="C221" s="9" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4251,21 +4273,21 @@
         <v>268</v>
       </c>
       <c r="B222" s="8" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="C222" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="223" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="7" t="s">
         <v>268</v>
       </c>
       <c r="B223" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="C223" s="6" t="s">
-        <v>119</v>
+        <v>282</v>
+      </c>
+      <c r="C223" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4273,21 +4295,21 @@
         <v>268</v>
       </c>
       <c r="B224" s="8" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="C224" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="225" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="7" t="s">
         <v>268</v>
       </c>
       <c r="B225" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="C225" s="6" t="s">
-        <v>119</v>
+        <v>284</v>
+      </c>
+      <c r="C225" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4295,10 +4317,10 @@
         <v>268</v>
       </c>
       <c r="B226" s="8" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="C226" s="6" t="s">
-        <v>119</v>
+        <v>286</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4306,21 +4328,21 @@
         <v>268</v>
       </c>
       <c r="B227" s="8" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="C227" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="228" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="7" t="s">
         <v>268</v>
       </c>
       <c r="B228" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="C228" s="6" t="s">
-        <v>119</v>
+        <v>288</v>
+      </c>
+      <c r="C228" s="9" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4328,10 +4350,10 @@
         <v>268</v>
       </c>
       <c r="B229" s="8" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="C229" s="6" t="s">
-        <v>119</v>
+        <v>10</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4339,21 +4361,21 @@
         <v>268</v>
       </c>
       <c r="B230" s="8" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="C230" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="231" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="231" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="7" t="s">
         <v>268</v>
       </c>
       <c r="B231" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="C231" s="6" t="s">
-        <v>119</v>
+        <v>292</v>
+      </c>
+      <c r="C231" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4361,10 +4383,10 @@
         <v>268</v>
       </c>
       <c r="B232" s="8" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="C232" s="6" t="s">
-        <v>119</v>
+        <v>8</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4372,32 +4394,32 @@
         <v>268</v>
       </c>
       <c r="B233" s="8" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="C233" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="234" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="7" t="s">
         <v>268</v>
       </c>
       <c r="B234" s="8" t="s">
-        <v>289</v>
-      </c>
-      <c r="C234" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="235" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>295</v>
+      </c>
+      <c r="C234" s="9" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="7" t="s">
         <v>268</v>
       </c>
       <c r="B235" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="C235" s="6" t="s">
-        <v>119</v>
+        <v>297</v>
+      </c>
+      <c r="C235" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4413,10 +4435,10 @@
     </row>
     <row r="238" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B238" s="8" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="C238" s="6" t="s">
         <v>119</v>
@@ -4424,10 +4446,10 @@
     </row>
     <row r="239" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B239" s="8" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="C239" s="6" t="s">
         <v>119</v>
@@ -4435,10 +4457,10 @@
     </row>
     <row r="240" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B240" s="8" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="C240" s="6" t="s">
         <v>119</v>
@@ -4446,10 +4468,10 @@
     </row>
     <row r="241" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B241" s="8" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="C241" s="6" t="s">
         <v>119</v>
@@ -4457,10 +4479,10 @@
     </row>
     <row r="242" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B242" s="8" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="C242" s="6" t="s">
         <v>119</v>
@@ -4468,10 +4490,10 @@
     </row>
     <row r="243" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B243" s="8" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="C243" s="6" t="s">
         <v>119</v>
@@ -4479,10 +4501,10 @@
     </row>
     <row r="244" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B244" s="8" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="C244" s="6" t="s">
         <v>119</v>
@@ -4490,10 +4512,10 @@
     </row>
     <row r="245" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B245" s="8" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="C245" s="6" t="s">
         <v>119</v>
@@ -4501,10 +4523,10 @@
     </row>
     <row r="246" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B246" s="8" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="C246" s="6" t="s">
         <v>119</v>
@@ -4512,10 +4534,10 @@
     </row>
     <row r="247" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B247" s="8" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="C247" s="6" t="s">
         <v>119</v>
@@ -4523,10 +4545,10 @@
     </row>
     <row r="248" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B248" s="8" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="C248" s="6" t="s">
         <v>119</v>
@@ -4534,10 +4556,10 @@
     </row>
     <row r="249" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B249" s="8" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="C249" s="6" t="s">
         <v>119</v>
@@ -4545,10 +4567,10 @@
     </row>
     <row r="250" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B250" s="8" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="C250" s="6" t="s">
         <v>119</v>
@@ -4556,10 +4578,10 @@
     </row>
     <row r="251" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B251" s="8" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="C251" s="6" t="s">
         <v>119</v>
@@ -4567,10 +4589,10 @@
     </row>
     <row r="252" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B252" s="8" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="C252" s="6" t="s">
         <v>119</v>
@@ -4578,10 +4600,10 @@
     </row>
     <row r="253" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B253" s="8" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="C253" s="6" t="s">
         <v>119</v>
@@ -4589,10 +4611,10 @@
     </row>
     <row r="254" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B254" s="8" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="C254" s="6" t="s">
         <v>119</v>
@@ -4600,10 +4622,10 @@
     </row>
     <row r="255" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B255" s="8" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="C255" s="6" t="s">
         <v>119</v>
@@ -4611,10 +4633,10 @@
     </row>
     <row r="256" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B256" s="8" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="C256" s="6" t="s">
         <v>119</v>
@@ -4622,10 +4644,10 @@
     </row>
     <row r="257" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B257" s="8" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="C257" s="6" t="s">
         <v>119</v>
@@ -4633,10 +4655,10 @@
     </row>
     <row r="258" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B258" s="8" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="C258" s="6" t="s">
         <v>119</v>
@@ -4644,10 +4666,10 @@
     </row>
     <row r="259" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B259" s="8" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C259" s="6" t="s">
         <v>119</v>
@@ -4655,10 +4677,10 @@
     </row>
     <row r="260" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B260" s="8" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="C260" s="6" t="s">
         <v>119</v>
@@ -4666,10 +4688,10 @@
     </row>
     <row r="261" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B261" s="8" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="C261" s="6" t="s">
         <v>119</v>
@@ -4677,10 +4699,10 @@
     </row>
     <row r="262" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B262" s="8" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="C262" s="6" t="s">
         <v>119</v>
@@ -4688,10 +4710,10 @@
     </row>
     <row r="263" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B263" s="8" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="C263" s="6" t="s">
         <v>119</v>
@@ -4699,10 +4721,10 @@
     </row>
     <row r="264" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B264" s="8" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="C264" s="6" t="s">
         <v>119</v>
@@ -4710,10 +4732,10 @@
     </row>
     <row r="265" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B265" s="8" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="C265" s="6" t="s">
         <v>119</v>
@@ -4721,10 +4743,10 @@
     </row>
     <row r="266" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B266" s="8" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="C266" s="6" t="s">
         <v>119</v>
@@ -4732,10 +4754,10 @@
     </row>
     <row r="267" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B267" s="8" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="C267" s="6" t="s">
         <v>119</v>
@@ -4743,10 +4765,10 @@
     </row>
     <row r="268" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B268" s="8" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="C268" s="6" t="s">
         <v>119</v>
@@ -4754,10 +4776,10 @@
     </row>
     <row r="269" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B269" s="8" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
       <c r="C269" s="6" t="s">
         <v>119</v>
@@ -4765,10 +4787,10 @@
     </row>
     <row r="270" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B270" s="8" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="C270" s="6" t="s">
         <v>119</v>
@@ -4776,7 +4798,7 @@
     </row>
     <row r="271" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B271" s="8" t="s">
         <v>120</v>
@@ -4787,10 +4809,10 @@
     </row>
     <row r="272" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="7" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="B272" s="8" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="C272" s="6" t="s">
         <v>119</v>
@@ -4802,17 +4824,17 @@
     </row>
     <row r="274" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="0" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B274" s="10"/>
       <c r="C274" s="6"/>
     </row>
     <row r="275" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="B275" s="8" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="C275" s="6" t="s">
         <v>119</v>
@@ -4820,10 +4842,10 @@
     </row>
     <row r="276" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="B276" s="8" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="C276" s="6" t="s">
         <v>119</v>
@@ -4831,10 +4853,10 @@
     </row>
     <row r="277" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="B277" s="8" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
       <c r="C277" s="6" t="s">
         <v>119</v>
@@ -4842,10 +4864,10 @@
     </row>
     <row r="278" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="B278" s="8" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="C278" s="6" t="s">
         <v>119</v>
@@ -4853,10 +4875,10 @@
     </row>
     <row r="279" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="B279" s="8" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="C279" s="6" t="s">
         <v>119</v>
@@ -4864,10 +4886,10 @@
     </row>
     <row r="280" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="B280" s="8" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="C280" s="6" t="s">
         <v>119</v>
@@ -4875,10 +4897,10 @@
     </row>
     <row r="281" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="B281" s="8" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="C281" s="6" t="s">
         <v>119</v>
@@ -4886,10 +4908,10 @@
     </row>
     <row r="282" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="B282" s="8" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="C282" s="6" t="s">
         <v>119</v>
@@ -4897,10 +4919,10 @@
     </row>
     <row r="283" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="B283" s="8" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="C283" s="6" t="s">
         <v>119</v>
@@ -4908,10 +4930,10 @@
     </row>
     <row r="284" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="B284" s="8" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="C284" s="6" t="s">
         <v>119</v>
@@ -4919,10 +4941,10 @@
     </row>
     <row r="285" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="B285" s="8" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="C285" s="6" t="s">
         <v>119</v>
@@ -4930,10 +4952,10 @@
     </row>
     <row r="286" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="B286" s="8" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
       <c r="C286" s="6" t="s">
         <v>119</v>
@@ -4941,10 +4963,10 @@
     </row>
     <row r="287" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="B287" s="8" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="C287" s="6" t="s">
         <v>119</v>
@@ -4952,10 +4974,10 @@
     </row>
     <row r="288" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="B288" s="8" t="s">
-        <v>340</v>
+        <v>347</v>
       </c>
       <c r="C288" s="6" t="s">
         <v>119</v>
@@ -4963,10 +4985,10 @@
     </row>
     <row r="289" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="B289" s="8" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="C289" s="6" t="s">
         <v>119</v>
@@ -4974,10 +4996,10 @@
     </row>
     <row r="290" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="B290" s="8" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="C290" s="6" t="s">
         <v>119</v>
@@ -4985,10 +5007,10 @@
     </row>
     <row r="291" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="B291" s="8" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="C291" s="6" t="s">
         <v>119</v>
@@ -4996,10 +5018,10 @@
     </row>
     <row r="292" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="B292" s="8" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="C292" s="6" t="s">
         <v>119</v>
@@ -5007,10 +5029,10 @@
     </row>
     <row r="293" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="7" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="B293" s="8" t="s">
-        <v>345</v>
+        <v>352</v>
       </c>
       <c r="C293" s="6" t="s">
         <v>119</v>
@@ -5029,10 +5051,10 @@
     </row>
     <row r="296" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B296" s="8" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
       <c r="C296" s="6" t="s">
         <v>119</v>
@@ -5040,10 +5062,10 @@
     </row>
     <row r="297" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B297" s="8" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="C297" s="6" t="s">
         <v>119</v>
@@ -5051,10 +5073,10 @@
     </row>
     <row r="298" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B298" s="8" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
       <c r="C298" s="6" t="s">
         <v>119</v>
@@ -5062,10 +5084,10 @@
     </row>
     <row r="299" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B299" s="8" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="C299" s="6" t="s">
         <v>119</v>
@@ -5073,10 +5095,10 @@
     </row>
     <row r="300" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B300" s="8" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="C300" s="6" t="s">
         <v>119</v>
@@ -5084,10 +5106,10 @@
     </row>
     <row r="301" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B301" s="8" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="C301" s="6" t="s">
         <v>119</v>
@@ -5095,10 +5117,10 @@
     </row>
     <row r="302" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B302" s="8" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="C302" s="6" t="s">
         <v>119</v>
@@ -5106,10 +5128,10 @@
     </row>
     <row r="303" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B303" s="8" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="C303" s="6" t="s">
         <v>119</v>
@@ -5117,10 +5139,10 @@
     </row>
     <row r="304" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B304" s="8" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
       <c r="C304" s="6" t="s">
         <v>119</v>
@@ -5128,10 +5150,10 @@
     </row>
     <row r="305" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B305" s="8" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="C305" s="6" t="s">
         <v>119</v>
@@ -5139,10 +5161,10 @@
     </row>
     <row r="306" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B306" s="8" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="C306" s="6" t="s">
         <v>119</v>
@@ -5150,10 +5172,10 @@
     </row>
     <row r="307" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B307" s="8" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="C307" s="6" t="s">
         <v>119</v>
@@ -5161,10 +5183,10 @@
     </row>
     <row r="308" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B308" s="8" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="C308" s="6" t="s">
         <v>119</v>
@@ -5172,10 +5194,10 @@
     </row>
     <row r="309" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B309" s="12" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="C309" s="6" t="s">
         <v>119</v>
@@ -5183,10 +5205,10 @@
     </row>
     <row r="310" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B310" s="8" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="C310" s="6" t="s">
         <v>119</v>
@@ -5194,10 +5216,10 @@
     </row>
     <row r="311" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B311" s="8" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="C311" s="6" t="s">
         <v>119</v>
@@ -5205,10 +5227,10 @@
     </row>
     <row r="312" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B312" s="8" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="C312" s="6" t="s">
         <v>119</v>
@@ -5216,10 +5238,10 @@
     </row>
     <row r="313" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B313" s="8" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="C313" s="6" t="s">
         <v>119</v>
@@ -5227,10 +5249,10 @@
     </row>
     <row r="314" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B314" s="8" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="C314" s="6" t="s">
         <v>119</v>
@@ -5238,10 +5260,10 @@
     </row>
     <row r="315" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B315" s="8" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="C315" s="6" t="s">
         <v>119</v>
@@ -5249,10 +5271,10 @@
     </row>
     <row r="316" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B316" s="8" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="C316" s="6" t="s">
         <v>119</v>
@@ -5260,10 +5282,10 @@
     </row>
     <row r="317" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B317" s="8" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="C317" s="6" t="s">
         <v>119</v>
@@ -5271,10 +5293,10 @@
     </row>
     <row r="318" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B318" s="8" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="C318" s="6" t="s">
         <v>119</v>
@@ -5282,10 +5304,10 @@
     </row>
     <row r="319" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B319" s="8" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="C319" s="6" t="s">
         <v>119</v>
@@ -5293,10 +5315,10 @@
     </row>
     <row r="320" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B320" s="8" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="C320" s="6" t="s">
         <v>119</v>
@@ -5304,10 +5326,10 @@
     </row>
     <row r="321" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B321" s="8" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="C321" s="6" t="s">
         <v>119</v>
@@ -5315,10 +5337,10 @@
     </row>
     <row r="322" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B322" s="8" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="C322" s="6" t="s">
         <v>119</v>
@@ -5326,10 +5348,10 @@
     </row>
     <row r="323" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B323" s="8" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
       <c r="C323" s="6" t="s">
         <v>119</v>
@@ -5337,10 +5359,10 @@
     </row>
     <row r="324" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B324" s="8" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="C324" s="6" t="s">
         <v>119</v>
@@ -5348,10 +5370,10 @@
     </row>
     <row r="325" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B325" s="8" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="C325" s="6" t="s">
         <v>119</v>
@@ -5359,10 +5381,10 @@
     </row>
     <row r="326" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B326" s="8" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="C326" s="6" t="s">
         <v>119</v>
@@ -5370,10 +5392,10 @@
     </row>
     <row r="327" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B327" s="8" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="C327" s="6" t="s">
         <v>119</v>
@@ -5381,10 +5403,10 @@
     </row>
     <row r="328" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B328" s="8" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
       <c r="C328" s="6" t="s">
         <v>119</v>
@@ -5392,10 +5414,10 @@
     </row>
     <row r="329" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B329" s="8" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="C329" s="6" t="s">
         <v>119</v>
@@ -5403,10 +5425,10 @@
     </row>
     <row r="330" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B330" s="8" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="C330" s="6" t="s">
         <v>119</v>
@@ -5414,10 +5436,10 @@
     </row>
     <row r="331" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B331" s="8" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
       <c r="C331" s="6" t="s">
         <v>119</v>
@@ -5425,10 +5447,10 @@
     </row>
     <row r="332" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B332" s="8" t="s">
-        <v>383</v>
+        <v>390</v>
       </c>
       <c r="C332" s="6" t="s">
         <v>119</v>
@@ -5436,10 +5458,10 @@
     </row>
     <row r="333" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="7" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B333" s="8" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="C333" s="6" t="s">
         <v>119</v>
@@ -5458,10 +5480,10 @@
     </row>
     <row r="336" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="7" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="B336" s="8" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
       <c r="C336" s="6" t="s">
         <v>119</v>
@@ -5469,10 +5491,10 @@
     </row>
     <row r="337" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="7" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="B337" s="8" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
       <c r="C337" s="6" t="s">
         <v>119</v>
@@ -5480,10 +5502,10 @@
     </row>
     <row r="338" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="7" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="B338" s="8" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
       <c r="C338" s="6" t="s">
         <v>119</v>
@@ -5491,10 +5513,10 @@
     </row>
     <row r="339" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="7" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="B339" s="8" t="s">
-        <v>389</v>
+        <v>396</v>
       </c>
       <c r="C339" s="6" t="s">
         <v>119</v>
@@ -5502,10 +5524,10 @@
     </row>
     <row r="340" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="7" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="B340" s="8" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
       <c r="C340" s="6" t="s">
         <v>119</v>
@@ -5513,10 +5535,10 @@
     </row>
     <row r="341" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="7" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="B341" s="8" t="s">
-        <v>391</v>
+        <v>398</v>
       </c>
       <c r="C341" s="6" t="s">
         <v>119</v>
@@ -5524,10 +5546,10 @@
     </row>
     <row r="342" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="7" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="B342" s="8" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
       <c r="C342" s="6" t="s">
         <v>119</v>
@@ -5535,10 +5557,10 @@
     </row>
     <row r="343" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="7" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="B343" s="8" t="s">
-        <v>393</v>
+        <v>400</v>
       </c>
       <c r="C343" s="6" t="s">
         <v>119</v>
@@ -5546,10 +5568,10 @@
     </row>
     <row r="344" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="7" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="B344" s="12" t="s">
-        <v>394</v>
+        <v>401</v>
       </c>
       <c r="C344" s="6" t="s">
         <v>119</v>
@@ -5557,10 +5579,10 @@
     </row>
     <row r="345" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="7" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="B345" s="8" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C345" s="6" t="s">
         <v>119</v>
@@ -5568,10 +5590,10 @@
     </row>
     <row r="346" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="7" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="B346" s="8" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="C346" s="6" t="s">
         <v>119</v>
@@ -5579,10 +5601,10 @@
     </row>
     <row r="347" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="7" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="B347" s="8" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="C347" s="6" t="s">
         <v>119</v>
@@ -5590,10 +5612,10 @@
     </row>
     <row r="348" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="7" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="B348" s="8" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
       <c r="C348" s="6" t="s">
         <v>119</v>
@@ -5601,10 +5623,10 @@
     </row>
     <row r="349" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="7" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="B349" s="8" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="C349" s="6" t="s">
         <v>119</v>
@@ -5612,10 +5634,10 @@
     </row>
     <row r="350" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="7" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="B350" s="8" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="C350" s="6" t="s">
         <v>119</v>
@@ -5623,10 +5645,10 @@
     </row>
     <row r="351" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="7" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="B351" s="8" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
       <c r="C351" s="6" t="s">
         <v>119</v>
@@ -5634,10 +5656,10 @@
     </row>
     <row r="352" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="7" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="B352" s="8" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="C352" s="6" t="s">
         <v>119</v>
@@ -5645,10 +5667,10 @@
     </row>
     <row r="353" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="7" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="B353" s="8" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="C353" s="6" t="s">
         <v>119</v>
@@ -5667,10 +5689,10 @@
     </row>
     <row r="356" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B356" s="8" t="s">
-        <v>405</v>
+        <v>412</v>
       </c>
       <c r="C356" s="6" t="s">
         <v>119</v>
@@ -5678,10 +5700,10 @@
     </row>
     <row r="357" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B357" s="8" t="s">
-        <v>406</v>
+        <v>413</v>
       </c>
       <c r="C357" s="6" t="s">
         <v>119</v>
@@ -5689,10 +5711,10 @@
     </row>
     <row r="358" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B358" s="8" t="s">
-        <v>407</v>
+        <v>414</v>
       </c>
       <c r="C358" s="6" t="s">
         <v>119</v>
@@ -5700,10 +5722,10 @@
     </row>
     <row r="359" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B359" s="8" t="s">
-        <v>408</v>
+        <v>415</v>
       </c>
       <c r="C359" s="6" t="s">
         <v>119</v>
@@ -5711,10 +5733,10 @@
     </row>
     <row r="360" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B360" s="8" t="s">
-        <v>409</v>
+        <v>416</v>
       </c>
       <c r="C360" s="6" t="s">
         <v>119</v>
@@ -5722,10 +5744,10 @@
     </row>
     <row r="361" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B361" s="8" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="C361" s="6" t="s">
         <v>119</v>
@@ -5733,10 +5755,10 @@
     </row>
     <row r="362" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B362" s="8" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
       <c r="C362" s="6" t="s">
         <v>119</v>
@@ -5744,10 +5766,10 @@
     </row>
     <row r="363" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B363" s="8" t="s">
-        <v>412</v>
+        <v>419</v>
       </c>
       <c r="C363" s="6" t="s">
         <v>119</v>
@@ -5755,10 +5777,10 @@
     </row>
     <row r="364" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B364" s="8" t="s">
-        <v>413</v>
+        <v>420</v>
       </c>
       <c r="C364" s="6" t="s">
         <v>119</v>
@@ -5766,10 +5788,10 @@
     </row>
     <row r="365" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B365" s="8" t="s">
-        <v>414</v>
+        <v>421</v>
       </c>
       <c r="C365" s="6" t="s">
         <v>119</v>
@@ -5777,10 +5799,10 @@
     </row>
     <row r="366" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B366" s="8" t="s">
-        <v>415</v>
+        <v>422</v>
       </c>
       <c r="C366" s="6" t="s">
         <v>119</v>
@@ -5788,10 +5810,10 @@
     </row>
     <row r="367" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B367" s="8" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="C367" s="6" t="s">
         <v>119</v>
@@ -5799,10 +5821,10 @@
     </row>
     <row r="368" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B368" s="8" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
       <c r="C368" s="6" t="s">
         <v>119</v>
@@ -5810,10 +5832,10 @@
     </row>
     <row r="369" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B369" s="8" t="s">
-        <v>418</v>
+        <v>425</v>
       </c>
       <c r="C369" s="6" t="s">
         <v>119</v>
@@ -5821,10 +5843,10 @@
     </row>
     <row r="370" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B370" s="8" t="s">
-        <v>419</v>
+        <v>426</v>
       </c>
       <c r="C370" s="6" t="s">
         <v>119</v>
@@ -5832,10 +5854,10 @@
     </row>
     <row r="371" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B371" s="8" t="s">
-        <v>420</v>
+        <v>427</v>
       </c>
       <c r="C371" s="6" t="s">
         <v>119</v>
@@ -5843,10 +5865,10 @@
     </row>
     <row r="372" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B372" s="8" t="s">
-        <v>421</v>
+        <v>428</v>
       </c>
       <c r="C372" s="6" t="s">
         <v>119</v>
@@ -5854,10 +5876,10 @@
     </row>
     <row r="373" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B373" s="8" t="s">
-        <v>422</v>
+        <v>429</v>
       </c>
       <c r="C373" s="6" t="s">
         <v>119</v>
@@ -5865,10 +5887,10 @@
     </row>
     <row r="374" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B374" s="8" t="s">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="C374" s="6" t="s">
         <v>119</v>
@@ -5876,10 +5898,10 @@
     </row>
     <row r="375" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B375" s="8" t="s">
-        <v>424</v>
+        <v>431</v>
       </c>
       <c r="C375" s="6" t="s">
         <v>119</v>
@@ -5887,10 +5909,10 @@
     </row>
     <row r="376" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B376" s="8" t="s">
-        <v>425</v>
+        <v>432</v>
       </c>
       <c r="C376" s="6" t="s">
         <v>119</v>
@@ -5898,10 +5920,10 @@
     </row>
     <row r="377" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B377" s="8" t="s">
-        <v>426</v>
+        <v>433</v>
       </c>
       <c r="C377" s="6" t="s">
         <v>119</v>
@@ -5909,10 +5931,10 @@
     </row>
     <row r="378" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B378" s="8" t="s">
-        <v>427</v>
+        <v>434</v>
       </c>
       <c r="C378" s="6" t="s">
         <v>119</v>
@@ -5920,10 +5942,10 @@
     </row>
     <row r="379" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B379" s="8" t="s">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="C379" s="6" t="s">
         <v>119</v>
@@ -5931,10 +5953,10 @@
     </row>
     <row r="380" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B380" s="8" t="s">
-        <v>429</v>
+        <v>436</v>
       </c>
       <c r="C380" s="6" t="s">
         <v>119</v>
@@ -5942,10 +5964,10 @@
     </row>
     <row r="381" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B381" s="8" t="s">
-        <v>430</v>
+        <v>437</v>
       </c>
       <c r="C381" s="6" t="s">
         <v>119</v>
@@ -5953,10 +5975,10 @@
     </row>
     <row r="382" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B382" s="8" t="s">
-        <v>431</v>
+        <v>438</v>
       </c>
       <c r="C382" s="6" t="s">
         <v>119</v>
@@ -5964,10 +5986,10 @@
     </row>
     <row r="383" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B383" s="8" t="s">
-        <v>432</v>
+        <v>439</v>
       </c>
       <c r="C383" s="6" t="s">
         <v>119</v>
@@ -5975,10 +5997,10 @@
     </row>
     <row r="384" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B384" s="8" t="s">
-        <v>433</v>
+        <v>440</v>
       </c>
       <c r="C384" s="6" t="s">
         <v>119</v>
@@ -5986,10 +6008,10 @@
     </row>
     <row r="385" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B385" s="8" t="s">
-        <v>434</v>
+        <v>441</v>
       </c>
       <c r="C385" s="6" t="s">
         <v>119</v>
@@ -5997,10 +6019,10 @@
     </row>
     <row r="386" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B386" s="8" t="s">
-        <v>435</v>
+        <v>442</v>
       </c>
       <c r="C386" s="6" t="s">
         <v>119</v>
@@ -6008,10 +6030,10 @@
     </row>
     <row r="387" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B387" s="8" t="s">
-        <v>436</v>
+        <v>443</v>
       </c>
       <c r="C387" s="6" t="s">
         <v>119</v>
@@ -6019,10 +6041,10 @@
     </row>
     <row r="388" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B388" s="8" t="s">
-        <v>437</v>
+        <v>444</v>
       </c>
       <c r="C388" s="6" t="s">
         <v>119</v>
@@ -6030,10 +6052,10 @@
     </row>
     <row r="389" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B389" s="8" t="s">
-        <v>438</v>
+        <v>445</v>
       </c>
       <c r="C389" s="6" t="s">
         <v>119</v>
@@ -6041,10 +6063,10 @@
     </row>
     <row r="390" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B390" s="8" t="s">
-        <v>438</v>
+        <v>445</v>
       </c>
       <c r="C390" s="6" t="s">
         <v>119</v>
@@ -6052,10 +6074,10 @@
     </row>
     <row r="391" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B391" s="8" t="s">
-        <v>439</v>
+        <v>446</v>
       </c>
       <c r="C391" s="6" t="s">
         <v>119</v>
@@ -6063,10 +6085,10 @@
     </row>
     <row r="392" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B392" s="8" t="s">
-        <v>440</v>
+        <v>447</v>
       </c>
       <c r="C392" s="6" t="s">
         <v>119</v>
@@ -6074,10 +6096,10 @@
     </row>
     <row r="393" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B393" s="8" t="s">
-        <v>441</v>
+        <v>448</v>
       </c>
       <c r="C393" s="6" t="s">
         <v>119</v>
@@ -6085,10 +6107,10 @@
     </row>
     <row r="394" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B394" s="8" t="s">
-        <v>442</v>
+        <v>449</v>
       </c>
       <c r="C394" s="6" t="s">
         <v>119</v>
@@ -6096,10 +6118,10 @@
     </row>
     <row r="395" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B395" s="8" t="s">
-        <v>443</v>
+        <v>450</v>
       </c>
       <c r="C395" s="6" t="s">
         <v>119</v>
@@ -6107,10 +6129,10 @@
     </row>
     <row r="396" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B396" s="8" t="s">
-        <v>444</v>
+        <v>451</v>
       </c>
       <c r="C396" s="6" t="s">
         <v>119</v>
@@ -6118,10 +6140,10 @@
     </row>
     <row r="397" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B397" s="8" t="s">
-        <v>445</v>
+        <v>452</v>
       </c>
       <c r="C397" s="6" t="s">
         <v>119</v>
@@ -6129,10 +6151,10 @@
     </row>
     <row r="398" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B398" s="8" t="s">
-        <v>446</v>
+        <v>453</v>
       </c>
       <c r="C398" s="6" t="s">
         <v>119</v>
@@ -6140,10 +6162,10 @@
     </row>
     <row r="399" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="7" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B399" s="8" t="s">
-        <v>447</v>
+        <v>454</v>
       </c>
       <c r="C399" s="6" t="s">
         <v>119</v>
@@ -6162,10 +6184,10 @@
     </row>
     <row r="402" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="7" t="s">
-        <v>448</v>
+        <v>455</v>
       </c>
       <c r="B402" s="8" t="s">
-        <v>449</v>
+        <v>456</v>
       </c>
       <c r="C402" s="6" t="s">
         <v>119</v>
@@ -6173,10 +6195,10 @@
     </row>
     <row r="403" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="7" t="s">
-        <v>448</v>
+        <v>455</v>
       </c>
       <c r="B403" s="8" t="s">
-        <v>450</v>
+        <v>457</v>
       </c>
       <c r="C403" s="6" t="s">
         <v>119</v>
@@ -6184,10 +6206,10 @@
     </row>
     <row r="404" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="7" t="s">
-        <v>448</v>
+        <v>455</v>
       </c>
       <c r="B404" s="8" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
       <c r="C404" s="6" t="s">
         <v>119</v>
@@ -6195,7 +6217,7 @@
     </row>
     <row r="405" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="7" t="s">
-        <v>448</v>
+        <v>455</v>
       </c>
       <c r="B405" s="8" t="s">
         <v>122</v>
@@ -6206,10 +6228,10 @@
     </row>
     <row r="406" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="7" t="s">
-        <v>448</v>
+        <v>455</v>
       </c>
       <c r="B406" s="8" t="s">
-        <v>452</v>
+        <v>459</v>
       </c>
       <c r="C406" s="6" t="s">
         <v>119</v>
@@ -6217,10 +6239,10 @@
     </row>
     <row r="407" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="7" t="s">
-        <v>448</v>
+        <v>455</v>
       </c>
       <c r="B407" s="8" t="s">
-        <v>453</v>
+        <v>460</v>
       </c>
       <c r="C407" s="6" t="s">
         <v>119</v>
@@ -6239,10 +6261,10 @@
     </row>
     <row r="410" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B410" s="8" t="s">
-        <v>455</v>
+        <v>462</v>
       </c>
       <c r="C410" s="6" t="s">
         <v>119</v>
@@ -6250,10 +6272,10 @@
     </row>
     <row r="411" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B411" s="8" t="s">
-        <v>456</v>
+        <v>463</v>
       </c>
       <c r="C411" s="6" t="s">
         <v>119</v>
@@ -6261,10 +6283,10 @@
     </row>
     <row r="412" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B412" s="8" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="C412" s="6" t="s">
         <v>119</v>
@@ -6272,10 +6294,10 @@
     </row>
     <row r="413" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B413" s="8" t="s">
-        <v>458</v>
+        <v>465</v>
       </c>
       <c r="C413" s="6" t="s">
         <v>119</v>
@@ -6283,10 +6305,10 @@
     </row>
     <row r="414" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B414" s="8" t="s">
-        <v>459</v>
+        <v>466</v>
       </c>
       <c r="C414" s="6" t="s">
         <v>119</v>
@@ -6294,10 +6316,10 @@
     </row>
     <row r="415" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B415" s="8" t="s">
-        <v>460</v>
+        <v>467</v>
       </c>
       <c r="C415" s="6" t="s">
         <v>119</v>
@@ -6305,10 +6327,10 @@
     </row>
     <row r="416" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B416" s="8" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="C416" s="6" t="s">
         <v>119</v>
@@ -6316,10 +6338,10 @@
     </row>
     <row r="417" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B417" s="8" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="C417" s="6" t="s">
         <v>119</v>
@@ -6327,10 +6349,10 @@
     </row>
     <row r="418" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B418" s="8" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
       <c r="C418" s="6" t="s">
         <v>119</v>
@@ -6338,10 +6360,10 @@
     </row>
     <row r="419" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B419" s="8" t="s">
-        <v>463</v>
+        <v>470</v>
       </c>
       <c r="C419" s="6" t="s">
         <v>119</v>
@@ -6349,10 +6371,10 @@
     </row>
     <row r="420" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B420" s="8" t="s">
-        <v>464</v>
+        <v>471</v>
       </c>
       <c r="C420" s="6" t="s">
         <v>119</v>
@@ -6360,10 +6382,10 @@
     </row>
     <row r="421" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B421" s="8" t="s">
-        <v>465</v>
+        <v>472</v>
       </c>
       <c r="C421" s="6" t="s">
         <v>119</v>
@@ -6371,10 +6393,10 @@
     </row>
     <row r="422" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B422" s="8" t="s">
-        <v>466</v>
+        <v>473</v>
       </c>
       <c r="C422" s="6" t="s">
         <v>119</v>
@@ -6382,10 +6404,10 @@
     </row>
     <row r="423" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B423" s="8" t="s">
-        <v>467</v>
+        <v>474</v>
       </c>
       <c r="C423" s="6" t="s">
         <v>119</v>
@@ -6393,10 +6415,10 @@
     </row>
     <row r="424" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B424" s="8" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="C424" s="6" t="s">
         <v>119</v>
@@ -6404,10 +6426,10 @@
     </row>
     <row r="425" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B425" s="8" t="s">
-        <v>469</v>
+        <v>476</v>
       </c>
       <c r="C425" s="6" t="s">
         <v>119</v>
@@ -6415,10 +6437,10 @@
     </row>
     <row r="426" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B426" s="8" t="s">
-        <v>470</v>
+        <v>477</v>
       </c>
       <c r="C426" s="6" t="s">
         <v>119</v>
@@ -6426,10 +6448,10 @@
     </row>
     <row r="427" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B427" s="8" t="s">
-        <v>471</v>
+        <v>478</v>
       </c>
       <c r="C427" s="6" t="s">
         <v>119</v>
@@ -6437,10 +6459,10 @@
     </row>
     <row r="428" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B428" s="8" t="s">
-        <v>472</v>
+        <v>479</v>
       </c>
       <c r="C428" s="6" t="s">
         <v>119</v>
@@ -6448,10 +6470,10 @@
     </row>
     <row r="429" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B429" s="8" t="s">
-        <v>473</v>
+        <v>480</v>
       </c>
       <c r="C429" s="6" t="s">
         <v>119</v>
@@ -6459,10 +6481,10 @@
     </row>
     <row r="430" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B430" s="8" t="s">
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="C430" s="6" t="s">
         <v>119</v>
@@ -6470,10 +6492,10 @@
     </row>
     <row r="431" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B431" s="8" t="s">
-        <v>475</v>
+        <v>482</v>
       </c>
       <c r="C431" s="6" t="s">
         <v>119</v>
@@ -6481,10 +6503,10 @@
     </row>
     <row r="432" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B432" s="8" t="s">
-        <v>476</v>
+        <v>483</v>
       </c>
       <c r="C432" s="6" t="s">
         <v>119</v>
@@ -6492,10 +6514,10 @@
     </row>
     <row r="433" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B433" s="8" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
       <c r="C433" s="6" t="s">
         <v>119</v>
@@ -6503,10 +6525,10 @@
     </row>
     <row r="434" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B434" s="8" t="s">
-        <v>478</v>
+        <v>485</v>
       </c>
       <c r="C434" s="6" t="s">
         <v>119</v>
@@ -6514,10 +6536,10 @@
     </row>
     <row r="435" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B435" s="8" t="s">
-        <v>479</v>
+        <v>486</v>
       </c>
       <c r="C435" s="6" t="s">
         <v>119</v>
@@ -6525,10 +6547,10 @@
     </row>
     <row r="436" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B436" s="8" t="s">
-        <v>480</v>
+        <v>487</v>
       </c>
       <c r="C436" s="6" t="s">
         <v>119</v>
@@ -6536,10 +6558,10 @@
     </row>
     <row r="437" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B437" s="8" t="s">
-        <v>481</v>
+        <v>488</v>
       </c>
       <c r="C437" s="6" t="s">
         <v>119</v>
@@ -6547,10 +6569,10 @@
     </row>
     <row r="438" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B438" s="8" t="s">
-        <v>482</v>
+        <v>489</v>
       </c>
       <c r="C438" s="6" t="s">
         <v>119</v>
@@ -6558,10 +6580,10 @@
     </row>
     <row r="439" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B439" s="8" t="s">
-        <v>483</v>
+        <v>490</v>
       </c>
       <c r="C439" s="6" t="s">
         <v>119</v>
@@ -6569,10 +6591,10 @@
     </row>
     <row r="440" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B440" s="8" t="s">
-        <v>484</v>
+        <v>491</v>
       </c>
       <c r="C440" s="6" t="s">
         <v>119</v>
@@ -6580,10 +6602,10 @@
     </row>
     <row r="441" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B441" s="8" t="s">
-        <v>485</v>
+        <v>492</v>
       </c>
       <c r="C441" s="6" t="s">
         <v>119</v>
@@ -6591,10 +6613,10 @@
     </row>
     <row r="442" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B442" s="8" t="s">
-        <v>486</v>
+        <v>493</v>
       </c>
       <c r="C442" s="6" t="s">
         <v>119</v>
@@ -6602,10 +6624,10 @@
     </row>
     <row r="443" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B443" s="8" t="s">
-        <v>487</v>
+        <v>494</v>
       </c>
       <c r="C443" s="6" t="s">
         <v>119</v>
@@ -6613,10 +6635,10 @@
     </row>
     <row r="444" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B444" s="8" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="C444" s="6" t="s">
         <v>119</v>
@@ -6624,10 +6646,10 @@
     </row>
     <row r="445" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B445" s="8" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="C445" s="6" t="s">
         <v>119</v>
@@ -6635,10 +6657,10 @@
     </row>
     <row r="446" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B446" s="8" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="C446" s="6" t="s">
         <v>119</v>
@@ -6646,10 +6668,10 @@
     </row>
     <row r="447" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B447" s="8" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
       <c r="C447" s="6" t="s">
         <v>119</v>
@@ -6657,10 +6679,10 @@
     </row>
     <row r="448" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B448" s="8" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="C448" s="6" t="s">
         <v>119</v>
@@ -6668,10 +6690,10 @@
     </row>
     <row r="449" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B449" s="8" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="C449" s="6" t="s">
         <v>119</v>
@@ -6679,10 +6701,10 @@
     </row>
     <row r="450" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B450" s="8" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="C450" s="6" t="s">
         <v>119</v>
@@ -6690,10 +6712,10 @@
     </row>
     <row r="451" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B451" s="8" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="C451" s="6" t="s">
         <v>119</v>
@@ -6701,10 +6723,10 @@
     </row>
     <row r="452" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B452" s="8" t="s">
-        <v>496</v>
+        <v>503</v>
       </c>
       <c r="C452" s="6" t="s">
         <v>119</v>
@@ -6712,10 +6734,10 @@
     </row>
     <row r="453" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B453" s="8" t="s">
-        <v>497</v>
+        <v>504</v>
       </c>
       <c r="C453" s="6" t="s">
         <v>119</v>
@@ -6723,10 +6745,10 @@
     </row>
     <row r="454" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B454" s="8" t="s">
-        <v>498</v>
+        <v>505</v>
       </c>
       <c r="C454" s="6" t="s">
         <v>119</v>
@@ -6734,10 +6756,10 @@
     </row>
     <row r="455" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B455" s="8" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="C455" s="6" t="s">
         <v>119</v>
@@ -6745,10 +6767,10 @@
     </row>
     <row r="456" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B456" s="8" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="C456" s="6" t="s">
         <v>119</v>
@@ -6756,10 +6778,10 @@
     </row>
     <row r="457" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B457" s="8" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="C457" s="6" t="s">
         <v>119</v>
@@ -6767,10 +6789,10 @@
     </row>
     <row r="458" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B458" s="8" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="C458" s="6" t="s">
         <v>119</v>
@@ -6778,10 +6800,10 @@
     </row>
     <row r="459" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B459" s="8" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="C459" s="6" t="s">
         <v>119</v>
@@ -6789,10 +6811,10 @@
     </row>
     <row r="460" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B460" s="8" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="C460" s="6" t="s">
         <v>119</v>
@@ -6800,10 +6822,10 @@
     </row>
     <row r="461" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B461" s="8" t="s">
-        <v>505</v>
+        <v>512</v>
       </c>
       <c r="C461" s="6" t="s">
         <v>119</v>
@@ -6811,10 +6833,10 @@
     </row>
     <row r="462" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B462" s="8" t="s">
-        <v>506</v>
+        <v>513</v>
       </c>
       <c r="C462" s="6" t="s">
         <v>119</v>
@@ -6822,10 +6844,10 @@
     </row>
     <row r="463" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B463" s="8" t="s">
-        <v>507</v>
+        <v>514</v>
       </c>
       <c r="C463" s="6" t="s">
         <v>119</v>
@@ -6833,10 +6855,10 @@
     </row>
     <row r="464" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B464" s="8" t="s">
-        <v>508</v>
+        <v>515</v>
       </c>
       <c r="C464" s="6" t="s">
         <v>119</v>
@@ -6844,10 +6866,10 @@
     </row>
     <row r="465" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B465" s="8" t="s">
-        <v>509</v>
+        <v>516</v>
       </c>
       <c r="C465" s="6" t="s">
         <v>119</v>
@@ -6855,10 +6877,10 @@
     </row>
     <row r="466" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B466" s="8" t="s">
-        <v>510</v>
+        <v>517</v>
       </c>
       <c r="C466" s="6" t="s">
         <v>119</v>
@@ -6866,10 +6888,10 @@
     </row>
     <row r="467" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B467" s="8" t="s">
-        <v>511</v>
+        <v>518</v>
       </c>
       <c r="C467" s="6" t="s">
         <v>119</v>
@@ -6877,10 +6899,10 @@
     </row>
     <row r="468" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B468" s="8" t="s">
-        <v>512</v>
+        <v>519</v>
       </c>
       <c r="C468" s="6" t="s">
         <v>119</v>
@@ -6888,10 +6910,10 @@
     </row>
     <row r="469" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="7" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="B469" s="8" t="s">
-        <v>513</v>
+        <v>520</v>
       </c>
       <c r="C469" s="6" t="s">
         <v>119</v>
@@ -6910,10 +6932,10 @@
     </row>
     <row r="472" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="7" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="B472" s="8" t="s">
-        <v>515</v>
+        <v>522</v>
       </c>
       <c r="C472" s="6" t="s">
         <v>119</v>
@@ -6921,10 +6943,10 @@
     </row>
     <row r="473" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="7" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="B473" s="8" t="s">
-        <v>516</v>
+        <v>523</v>
       </c>
       <c r="C473" s="6" t="s">
         <v>119</v>
@@ -6932,10 +6954,10 @@
     </row>
     <row r="474" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="7" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="B474" s="8" t="s">
-        <v>517</v>
+        <v>524</v>
       </c>
       <c r="C474" s="6" t="s">
         <v>119</v>
@@ -6943,10 +6965,10 @@
     </row>
     <row r="475" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="7" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="B475" s="8" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="C475" s="6" t="s">
         <v>119</v>
@@ -6954,10 +6976,10 @@
     </row>
     <row r="476" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="7" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="B476" s="8" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
       <c r="C476" s="6" t="s">
         <v>119</v>
@@ -6965,10 +6987,10 @@
     </row>
     <row r="477" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="7" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="B477" s="8" t="s">
-        <v>520</v>
+        <v>527</v>
       </c>
       <c r="C477" s="6" t="s">
         <v>119</v>
@@ -6976,10 +6998,10 @@
     </row>
     <row r="478" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="7" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="B478" s="8" t="s">
-        <v>521</v>
+        <v>528</v>
       </c>
       <c r="C478" s="6" t="s">
         <v>119</v>
@@ -6987,10 +7009,10 @@
     </row>
     <row r="479" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="7" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="B479" s="8" t="s">
-        <v>522</v>
+        <v>529</v>
       </c>
       <c r="C479" s="6" t="s">
         <v>119</v>
@@ -6998,10 +7020,10 @@
     </row>
     <row r="480" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="7" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="B480" s="8" t="s">
-        <v>523</v>
+        <v>530</v>
       </c>
       <c r="C480" s="6" t="s">
         <v>119</v>
@@ -7009,10 +7031,10 @@
     </row>
     <row r="481" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="7" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="B481" s="8" t="s">
-        <v>524</v>
+        <v>531</v>
       </c>
       <c r="C481" s="6" t="s">
         <v>119</v>

</xml_diff>

<commit_message>
Graph added (except chinese postman)
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="574">
   <si>
     <t xml:space="preserve">YES(Iterative &amp; recursive)</t>
   </si>
@@ -1327,33 +1327,57 @@
     <t xml:space="preserve">Detect Cycle in Directed Graph using BFS/DFS Algo </t>
   </si>
   <si>
+    <t xml:space="preserve">YES(Recall DFS prcedure, BFS Kahn topo sort)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Detect Cycle in UnDirected Graph using BFS/DFS Algo </t>
   </si>
   <si>
+    <t xml:space="preserve">YES(DFS similarPrevious,BFS sameAsBFSalgo)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Search in a Maze</t>
   </si>
   <si>
     <t xml:space="preserve">Minimum Step by Knight</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(BFS and DP)</t>
+  </si>
+  <si>
     <t xml:space="preserve">flood fill algo</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(Recursion or BFS)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Clone a graph</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(DFS/BFS)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Making wired Connections</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(BFS/DFS or Union Find)</t>
+  </si>
+  <si>
     <t xml:space="preserve">word Ladder </t>
   </si>
   <si>
+    <t xml:space="preserve">YES(BFS)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dijkstra algo</t>
   </si>
   <si>
     <t xml:space="preserve">Implement Topological Sort </t>
   </si>
   <si>
+    <t xml:space="preserve">y(topology sorting Kahn’s Algo)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Minimum time taken by each job to be completed given by a Directed Acyclic Graph</t>
   </si>
   <si>
@@ -1363,18 +1387,33 @@
     <t xml:space="preserve">Find the no. of Isalnds</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(BFS/DFS or Union Find)bfs/dfs faster rn</t>
+  </si>
+  <si>
     <t xml:space="preserve">Given a sorted Dictionary of an Alien Language, find order of characters</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(make adj list and topological sort)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Implement Kruksal’sAlgorithm</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(Edge based)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Implement Prim’s Algorithm</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(node based)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Total no. of Spanning tree in a graph</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(Kirchhoff’s Theorem)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Implement Bellman Ford Algorithm</t>
   </si>
   <si>
@@ -1384,64 +1423,124 @@
     <t xml:space="preserve">Travelling Salesman Problem</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(permutation or DP)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Graph ColouringProblem</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(recall technique)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Snake and Ladders Problem</t>
   </si>
   <si>
+    <t xml:space="preserve">y(BFS)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Find bridge in a graph</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(tough, algo recall)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Count Strongly connected Components(Kosaraju Algo)</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(DFS,ReverseGraph,DFS)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Check whether a graph is Bipartite or Not</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(Graph Coloring)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Detect Negative cycle in a graph</t>
   </si>
   <si>
     <t xml:space="preserve">Longest path in a Directed Acyclic Graph</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(topological order)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Journey to the Moon</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(union find set/DFS to find components)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cheapest Flights Within K Stops</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(Modified Bellman Ford)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Oliver and the Game</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(DFS and inTime outTime)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Water Jug problem using BFS</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(3 possible neighbours)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Find if there is a path of more thank length from a source</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(DFS and Backtracking)</t>
+  </si>
+  <si>
     <t xml:space="preserve">M-ColouringProblem</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(using recursion)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Minimum edges to reverse o make path from source to destination</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(modify graph with reverse edge cost 1)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Paths to travel each nodes using each edge(Seven Bridges)</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(see method both directed &amp; indirected)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vertex Cover Problem</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(approximate method not actual answer)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chinese Postman or Route Inspection</t>
   </si>
   <si>
+    <t xml:space="preserve">INCOMPLETE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Number of Triangles in a Directed and Undirected Graph</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(count triplet or trace(A^3)/6)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Minimise the cashflow among a given set of friends who have borrowed money from each other</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(recursion give from maxCred to maxDeb)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Two Clique Problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES(complement and bipartite)</t>
   </si>
   <si>
     <t xml:space="preserve">Trie</t>
@@ -1956,11 +2055,11 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A334" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C354" activeCellId="0" sqref="C354"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A371" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C400" activeCellId="0" sqref="C400"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="111.76"/>
@@ -4856,15 +4955,15 @@
       <c r="B274" s="10"/>
       <c r="C274" s="6"/>
     </row>
-    <row r="275" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="275" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="7" t="s">
         <v>333</v>
       </c>
       <c r="B275" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="C275" s="6" t="s">
-        <v>119</v>
+      <c r="C275" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5626,7 +5725,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="347" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="347" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="7" t="s">
         <v>392</v>
       </c>
@@ -5721,8 +5820,8 @@
       <c r="B356" s="8" t="s">
         <v>421</v>
       </c>
-      <c r="C356" s="6" t="s">
-        <v>119</v>
+      <c r="C356" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5732,96 +5831,96 @@
       <c r="B357" s="8" t="s">
         <v>422</v>
       </c>
-      <c r="C357" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="358" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C357" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="358" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B358" s="8" t="s">
         <v>423</v>
       </c>
-      <c r="C358" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="359" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C358" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="359" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B359" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="C359" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="360" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C359" s="9" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="360" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B360" s="8" t="s">
-        <v>425</v>
-      </c>
-      <c r="C360" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="361" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>426</v>
+      </c>
+      <c r="C360" s="9" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="361" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B361" s="8" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="C361" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="362" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="362" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B362" s="8" t="s">
-        <v>427</v>
-      </c>
-      <c r="C362" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="363" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>429</v>
+      </c>
+      <c r="C362" s="9" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="363" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B363" s="8" t="s">
-        <v>428</v>
-      </c>
-      <c r="C363" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="364" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>431</v>
+      </c>
+      <c r="C363" s="9" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="364" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B364" s="8" t="s">
-        <v>429</v>
-      </c>
-      <c r="C364" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="365" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>433</v>
+      </c>
+      <c r="C364" s="9" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="365" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B365" s="8" t="s">
-        <v>430</v>
-      </c>
-      <c r="C365" s="6" t="s">
-        <v>119</v>
+        <v>435</v>
+      </c>
+      <c r="C365" s="9" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5829,153 +5928,153 @@
         <v>420</v>
       </c>
       <c r="B366" s="8" t="s">
-        <v>431</v>
+        <v>437</v>
       </c>
       <c r="C366" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="367" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="367" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B367" s="8" t="s">
-        <v>432</v>
-      </c>
-      <c r="C367" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="368" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>439</v>
+      </c>
+      <c r="C367" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="368" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B368" s="8" t="s">
-        <v>433</v>
+        <v>440</v>
       </c>
       <c r="C368" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="369" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="369" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B369" s="8" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="C369" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="370" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="370" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B370" s="8" t="s">
-        <v>435</v>
+        <v>443</v>
       </c>
       <c r="C370" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="371" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="371" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B371" s="8" t="s">
-        <v>436</v>
-      </c>
-      <c r="C371" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="372" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>444</v>
+      </c>
+      <c r="C371" s="9" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="372" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B372" s="8" t="s">
-        <v>437</v>
-      </c>
-      <c r="C372" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="373" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>446</v>
+      </c>
+      <c r="C372" s="9" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="373" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B373" s="8" t="s">
-        <v>438</v>
-      </c>
-      <c r="C373" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="374" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>448</v>
+      </c>
+      <c r="C373" s="9" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="374" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B374" s="8" t="s">
-        <v>439</v>
-      </c>
-      <c r="C374" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="375" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>450</v>
+      </c>
+      <c r="C374" s="9" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="375" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B375" s="8" t="s">
-        <v>440</v>
-      </c>
-      <c r="C375" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="376" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>452</v>
+      </c>
+      <c r="C375" s="9" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="376" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B376" s="8" t="s">
-        <v>441</v>
-      </c>
-      <c r="C376" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="377" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>454</v>
+      </c>
+      <c r="C376" s="9" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="377" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B377" s="8" t="s">
-        <v>442</v>
-      </c>
-      <c r="C377" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="378" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>455</v>
+      </c>
+      <c r="C377" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="378" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B378" s="8" t="s">
-        <v>443</v>
-      </c>
-      <c r="C378" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="379" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>456</v>
+      </c>
+      <c r="C378" s="9" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="379" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B379" s="8" t="s">
-        <v>444</v>
-      </c>
-      <c r="C379" s="6" t="s">
-        <v>119</v>
+        <v>458</v>
+      </c>
+      <c r="C379" s="9" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5983,43 +6082,43 @@
         <v>420</v>
       </c>
       <c r="B380" s="8" t="s">
-        <v>445</v>
+        <v>460</v>
       </c>
       <c r="C380" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="381" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="381" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B381" s="8" t="s">
-        <v>446</v>
-      </c>
-      <c r="C381" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="382" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>462</v>
+      </c>
+      <c r="C381" s="9" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="382" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B382" s="8" t="s">
-        <v>447</v>
-      </c>
-      <c r="C382" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="383" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>464</v>
+      </c>
+      <c r="C382" s="9" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="383" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B383" s="8" t="s">
-        <v>448</v>
-      </c>
-      <c r="C383" s="6" t="s">
-        <v>119</v>
+        <v>466</v>
+      </c>
+      <c r="C383" s="9" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6027,65 +6126,65 @@
         <v>420</v>
       </c>
       <c r="B384" s="8" t="s">
-        <v>449</v>
+        <v>468</v>
       </c>
       <c r="C384" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="385" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="385" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B385" s="8" t="s">
-        <v>450</v>
-      </c>
-      <c r="C385" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="386" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>469</v>
+      </c>
+      <c r="C385" s="9" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="386" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B386" s="8" t="s">
-        <v>451</v>
-      </c>
-      <c r="C386" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="387" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>471</v>
+      </c>
+      <c r="C386" s="9" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="387" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B387" s="8" t="s">
-        <v>452</v>
-      </c>
-      <c r="C387" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="388" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>473</v>
+      </c>
+      <c r="C387" s="9" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="388" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B388" s="8" t="s">
-        <v>453</v>
-      </c>
-      <c r="C388" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="389" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>475</v>
+      </c>
+      <c r="C388" s="9" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="389" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B389" s="8" t="s">
-        <v>454</v>
-      </c>
-      <c r="C389" s="6" t="s">
-        <v>119</v>
+        <v>477</v>
+      </c>
+      <c r="C389" s="9" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6093,109 +6192,109 @@
         <v>420</v>
       </c>
       <c r="B390" s="8" t="s">
-        <v>454</v>
+        <v>477</v>
       </c>
       <c r="C390" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="391" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="391" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B391" s="8" t="s">
-        <v>455</v>
-      </c>
-      <c r="C391" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="392" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>479</v>
+      </c>
+      <c r="C391" s="9" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="392" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B392" s="8" t="s">
-        <v>456</v>
-      </c>
-      <c r="C392" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="393" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>481</v>
+      </c>
+      <c r="C392" s="9" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="393" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B393" s="8" t="s">
-        <v>457</v>
-      </c>
-      <c r="C393" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="394" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>483</v>
+      </c>
+      <c r="C393" s="9" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="394" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B394" s="8" t="s">
-        <v>458</v>
-      </c>
-      <c r="C394" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="395" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>485</v>
+      </c>
+      <c r="C394" s="9" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="395" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B395" s="8" t="s">
-        <v>459</v>
-      </c>
-      <c r="C395" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="396" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>487</v>
+      </c>
+      <c r="C395" s="9" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="396" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B396" s="8" t="s">
-        <v>460</v>
-      </c>
-      <c r="C396" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="397" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>489</v>
+      </c>
+      <c r="C396" s="11" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="397" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B397" s="8" t="s">
-        <v>461</v>
-      </c>
-      <c r="C397" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="398" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>491</v>
+      </c>
+      <c r="C397" s="9" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="398" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B398" s="8" t="s">
-        <v>462</v>
-      </c>
-      <c r="C398" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="399" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>493</v>
+      </c>
+      <c r="C398" s="9" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="399" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="7" t="s">
         <v>420</v>
       </c>
       <c r="B399" s="8" t="s">
-        <v>463</v>
-      </c>
-      <c r="C399" s="6" t="s">
-        <v>119</v>
+        <v>495</v>
+      </c>
+      <c r="C399" s="9" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6211,10 +6310,10 @@
     </row>
     <row r="402" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="7" t="s">
-        <v>464</v>
+        <v>497</v>
       </c>
       <c r="B402" s="8" t="s">
-        <v>465</v>
+        <v>498</v>
       </c>
       <c r="C402" s="6" t="s">
         <v>119</v>
@@ -6222,10 +6321,10 @@
     </row>
     <row r="403" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="7" t="s">
-        <v>464</v>
+        <v>497</v>
       </c>
       <c r="B403" s="8" t="s">
-        <v>466</v>
+        <v>499</v>
       </c>
       <c r="C403" s="6" t="s">
         <v>119</v>
@@ -6233,10 +6332,10 @@
     </row>
     <row r="404" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="7" t="s">
-        <v>464</v>
+        <v>497</v>
       </c>
       <c r="B404" s="8" t="s">
-        <v>467</v>
+        <v>500</v>
       </c>
       <c r="C404" s="6" t="s">
         <v>119</v>
@@ -6244,7 +6343,7 @@
     </row>
     <row r="405" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="7" t="s">
-        <v>464</v>
+        <v>497</v>
       </c>
       <c r="B405" s="8" t="s">
         <v>122</v>
@@ -6255,10 +6354,10 @@
     </row>
     <row r="406" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="7" t="s">
-        <v>464</v>
+        <v>497</v>
       </c>
       <c r="B406" s="8" t="s">
-        <v>468</v>
+        <v>501</v>
       </c>
       <c r="C406" s="6" t="s">
         <v>119</v>
@@ -6266,10 +6365,10 @@
     </row>
     <row r="407" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="7" t="s">
-        <v>464</v>
+        <v>497</v>
       </c>
       <c r="B407" s="8" t="s">
-        <v>469</v>
+        <v>502</v>
       </c>
       <c r="C407" s="6" t="s">
         <v>119</v>
@@ -6288,10 +6387,10 @@
     </row>
     <row r="410" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B410" s="8" t="s">
-        <v>471</v>
+        <v>504</v>
       </c>
       <c r="C410" s="6" t="s">
         <v>119</v>
@@ -6299,10 +6398,10 @@
     </row>
     <row r="411" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B411" s="8" t="s">
-        <v>472</v>
+        <v>505</v>
       </c>
       <c r="C411" s="6" t="s">
         <v>119</v>
@@ -6310,10 +6409,10 @@
     </row>
     <row r="412" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B412" s="8" t="s">
-        <v>473</v>
+        <v>506</v>
       </c>
       <c r="C412" s="6" t="s">
         <v>119</v>
@@ -6321,10 +6420,10 @@
     </row>
     <row r="413" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B413" s="8" t="s">
-        <v>474</v>
+        <v>507</v>
       </c>
       <c r="C413" s="6" t="s">
         <v>119</v>
@@ -6332,10 +6431,10 @@
     </row>
     <row r="414" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B414" s="8" t="s">
-        <v>475</v>
+        <v>508</v>
       </c>
       <c r="C414" s="6" t="s">
         <v>119</v>
@@ -6343,10 +6442,10 @@
     </row>
     <row r="415" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B415" s="8" t="s">
-        <v>476</v>
+        <v>509</v>
       </c>
       <c r="C415" s="6" t="s">
         <v>119</v>
@@ -6354,10 +6453,10 @@
     </row>
     <row r="416" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B416" s="8" t="s">
-        <v>477</v>
+        <v>510</v>
       </c>
       <c r="C416" s="6" t="s">
         <v>119</v>
@@ -6365,7 +6464,7 @@
     </row>
     <row r="417" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B417" s="8" t="s">
         <v>341</v>
@@ -6376,10 +6475,10 @@
     </row>
     <row r="418" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B418" s="8" t="s">
-        <v>478</v>
+        <v>511</v>
       </c>
       <c r="C418" s="6" t="s">
         <v>119</v>
@@ -6387,10 +6486,10 @@
     </row>
     <row r="419" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B419" s="8" t="s">
-        <v>479</v>
+        <v>512</v>
       </c>
       <c r="C419" s="6" t="s">
         <v>119</v>
@@ -6398,10 +6497,10 @@
     </row>
     <row r="420" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B420" s="8" t="s">
-        <v>480</v>
+        <v>513</v>
       </c>
       <c r="C420" s="6" t="s">
         <v>119</v>
@@ -6409,10 +6508,10 @@
     </row>
     <row r="421" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B421" s="8" t="s">
-        <v>481</v>
+        <v>514</v>
       </c>
       <c r="C421" s="6" t="s">
         <v>119</v>
@@ -6420,10 +6519,10 @@
     </row>
     <row r="422" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B422" s="8" t="s">
-        <v>482</v>
+        <v>515</v>
       </c>
       <c r="C422" s="6" t="s">
         <v>119</v>
@@ -6431,10 +6530,10 @@
     </row>
     <row r="423" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B423" s="8" t="s">
-        <v>483</v>
+        <v>516</v>
       </c>
       <c r="C423" s="6" t="s">
         <v>119</v>
@@ -6442,10 +6541,10 @@
     </row>
     <row r="424" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B424" s="8" t="s">
-        <v>484</v>
+        <v>517</v>
       </c>
       <c r="C424" s="6" t="s">
         <v>119</v>
@@ -6453,10 +6552,10 @@
     </row>
     <row r="425" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B425" s="8" t="s">
-        <v>485</v>
+        <v>518</v>
       </c>
       <c r="C425" s="6" t="s">
         <v>119</v>
@@ -6464,10 +6563,10 @@
     </row>
     <row r="426" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B426" s="8" t="s">
-        <v>486</v>
+        <v>519</v>
       </c>
       <c r="C426" s="6" t="s">
         <v>119</v>
@@ -6475,10 +6574,10 @@
     </row>
     <row r="427" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B427" s="8" t="s">
-        <v>487</v>
+        <v>520</v>
       </c>
       <c r="C427" s="6" t="s">
         <v>119</v>
@@ -6486,10 +6585,10 @@
     </row>
     <row r="428" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B428" s="8" t="s">
-        <v>488</v>
+        <v>521</v>
       </c>
       <c r="C428" s="6" t="s">
         <v>119</v>
@@ -6497,10 +6596,10 @@
     </row>
     <row r="429" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B429" s="8" t="s">
-        <v>489</v>
+        <v>522</v>
       </c>
       <c r="C429" s="6" t="s">
         <v>119</v>
@@ -6508,10 +6607,10 @@
     </row>
     <row r="430" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B430" s="8" t="s">
-        <v>490</v>
+        <v>523</v>
       </c>
       <c r="C430" s="6" t="s">
         <v>119</v>
@@ -6519,10 +6618,10 @@
     </row>
     <row r="431" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B431" s="8" t="s">
-        <v>491</v>
+        <v>524</v>
       </c>
       <c r="C431" s="6" t="s">
         <v>119</v>
@@ -6530,10 +6629,10 @@
     </row>
     <row r="432" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B432" s="8" t="s">
-        <v>492</v>
+        <v>525</v>
       </c>
       <c r="C432" s="6" t="s">
         <v>119</v>
@@ -6541,10 +6640,10 @@
     </row>
     <row r="433" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B433" s="8" t="s">
-        <v>493</v>
+        <v>526</v>
       </c>
       <c r="C433" s="6" t="s">
         <v>119</v>
@@ -6552,10 +6651,10 @@
     </row>
     <row r="434" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B434" s="8" t="s">
-        <v>494</v>
+        <v>527</v>
       </c>
       <c r="C434" s="6" t="s">
         <v>119</v>
@@ -6563,10 +6662,10 @@
     </row>
     <row r="435" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B435" s="8" t="s">
-        <v>495</v>
+        <v>528</v>
       </c>
       <c r="C435" s="6" t="s">
         <v>119</v>
@@ -6574,10 +6673,10 @@
     </row>
     <row r="436" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B436" s="8" t="s">
-        <v>496</v>
+        <v>529</v>
       </c>
       <c r="C436" s="6" t="s">
         <v>119</v>
@@ -6585,10 +6684,10 @@
     </row>
     <row r="437" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B437" s="8" t="s">
-        <v>497</v>
+        <v>530</v>
       </c>
       <c r="C437" s="6" t="s">
         <v>119</v>
@@ -6596,10 +6695,10 @@
     </row>
     <row r="438" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B438" s="8" t="s">
-        <v>498</v>
+        <v>531</v>
       </c>
       <c r="C438" s="6" t="s">
         <v>119</v>
@@ -6607,10 +6706,10 @@
     </row>
     <row r="439" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B439" s="8" t="s">
-        <v>499</v>
+        <v>532</v>
       </c>
       <c r="C439" s="6" t="s">
         <v>119</v>
@@ -6618,10 +6717,10 @@
     </row>
     <row r="440" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B440" s="8" t="s">
-        <v>500</v>
+        <v>533</v>
       </c>
       <c r="C440" s="6" t="s">
         <v>119</v>
@@ -6629,10 +6728,10 @@
     </row>
     <row r="441" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B441" s="8" t="s">
-        <v>501</v>
+        <v>534</v>
       </c>
       <c r="C441" s="6" t="s">
         <v>119</v>
@@ -6640,10 +6739,10 @@
     </row>
     <row r="442" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B442" s="8" t="s">
-        <v>502</v>
+        <v>535</v>
       </c>
       <c r="C442" s="6" t="s">
         <v>119</v>
@@ -6651,10 +6750,10 @@
     </row>
     <row r="443" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B443" s="8" t="s">
-        <v>503</v>
+        <v>536</v>
       </c>
       <c r="C443" s="6" t="s">
         <v>119</v>
@@ -6662,10 +6761,10 @@
     </row>
     <row r="444" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B444" s="8" t="s">
-        <v>504</v>
+        <v>537</v>
       </c>
       <c r="C444" s="6" t="s">
         <v>119</v>
@@ -6673,10 +6772,10 @@
     </row>
     <row r="445" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B445" s="8" t="s">
-        <v>505</v>
+        <v>538</v>
       </c>
       <c r="C445" s="6" t="s">
         <v>119</v>
@@ -6684,10 +6783,10 @@
     </row>
     <row r="446" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B446" s="8" t="s">
-        <v>506</v>
+        <v>539</v>
       </c>
       <c r="C446" s="6" t="s">
         <v>119</v>
@@ -6695,10 +6794,10 @@
     </row>
     <row r="447" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B447" s="8" t="s">
-        <v>507</v>
+        <v>540</v>
       </c>
       <c r="C447" s="6" t="s">
         <v>119</v>
@@ -6706,10 +6805,10 @@
     </row>
     <row r="448" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B448" s="8" t="s">
-        <v>508</v>
+        <v>541</v>
       </c>
       <c r="C448" s="6" t="s">
         <v>119</v>
@@ -6717,10 +6816,10 @@
     </row>
     <row r="449" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B449" s="8" t="s">
-        <v>509</v>
+        <v>542</v>
       </c>
       <c r="C449" s="6" t="s">
         <v>119</v>
@@ -6728,10 +6827,10 @@
     </row>
     <row r="450" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B450" s="8" t="s">
-        <v>510</v>
+        <v>543</v>
       </c>
       <c r="C450" s="6" t="s">
         <v>119</v>
@@ -6739,10 +6838,10 @@
     </row>
     <row r="451" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B451" s="8" t="s">
-        <v>511</v>
+        <v>544</v>
       </c>
       <c r="C451" s="6" t="s">
         <v>119</v>
@@ -6750,10 +6849,10 @@
     </row>
     <row r="452" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B452" s="8" t="s">
-        <v>512</v>
+        <v>545</v>
       </c>
       <c r="C452" s="6" t="s">
         <v>119</v>
@@ -6761,10 +6860,10 @@
     </row>
     <row r="453" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B453" s="8" t="s">
-        <v>513</v>
+        <v>546</v>
       </c>
       <c r="C453" s="6" t="s">
         <v>119</v>
@@ -6772,10 +6871,10 @@
     </row>
     <row r="454" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B454" s="8" t="s">
-        <v>514</v>
+        <v>547</v>
       </c>
       <c r="C454" s="6" t="s">
         <v>119</v>
@@ -6783,10 +6882,10 @@
     </row>
     <row r="455" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B455" s="8" t="s">
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="C455" s="6" t="s">
         <v>119</v>
@@ -6794,10 +6893,10 @@
     </row>
     <row r="456" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B456" s="8" t="s">
-        <v>516</v>
+        <v>549</v>
       </c>
       <c r="C456" s="6" t="s">
         <v>119</v>
@@ -6805,10 +6904,10 @@
     </row>
     <row r="457" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B457" s="8" t="s">
-        <v>517</v>
+        <v>550</v>
       </c>
       <c r="C457" s="6" t="s">
         <v>119</v>
@@ -6816,10 +6915,10 @@
     </row>
     <row r="458" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B458" s="8" t="s">
-        <v>518</v>
+        <v>551</v>
       </c>
       <c r="C458" s="6" t="s">
         <v>119</v>
@@ -6827,10 +6926,10 @@
     </row>
     <row r="459" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B459" s="8" t="s">
-        <v>519</v>
+        <v>552</v>
       </c>
       <c r="C459" s="6" t="s">
         <v>119</v>
@@ -6838,10 +6937,10 @@
     </row>
     <row r="460" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B460" s="8" t="s">
-        <v>520</v>
+        <v>553</v>
       </c>
       <c r="C460" s="6" t="s">
         <v>119</v>
@@ -6849,10 +6948,10 @@
     </row>
     <row r="461" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B461" s="8" t="s">
-        <v>521</v>
+        <v>554</v>
       </c>
       <c r="C461" s="6" t="s">
         <v>119</v>
@@ -6860,10 +6959,10 @@
     </row>
     <row r="462" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B462" s="8" t="s">
-        <v>522</v>
+        <v>555</v>
       </c>
       <c r="C462" s="6" t="s">
         <v>119</v>
@@ -6871,10 +6970,10 @@
     </row>
     <row r="463" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B463" s="8" t="s">
-        <v>523</v>
+        <v>556</v>
       </c>
       <c r="C463" s="6" t="s">
         <v>119</v>
@@ -6882,10 +6981,10 @@
     </row>
     <row r="464" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B464" s="8" t="s">
-        <v>524</v>
+        <v>557</v>
       </c>
       <c r="C464" s="6" t="s">
         <v>119</v>
@@ -6893,10 +6992,10 @@
     </row>
     <row r="465" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B465" s="8" t="s">
-        <v>525</v>
+        <v>558</v>
       </c>
       <c r="C465" s="6" t="s">
         <v>119</v>
@@ -6904,10 +7003,10 @@
     </row>
     <row r="466" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B466" s="8" t="s">
-        <v>526</v>
+        <v>559</v>
       </c>
       <c r="C466" s="6" t="s">
         <v>119</v>
@@ -6915,10 +7014,10 @@
     </row>
     <row r="467" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B467" s="8" t="s">
-        <v>527</v>
+        <v>560</v>
       </c>
       <c r="C467" s="6" t="s">
         <v>119</v>
@@ -6926,10 +7025,10 @@
     </row>
     <row r="468" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B468" s="8" t="s">
-        <v>528</v>
+        <v>561</v>
       </c>
       <c r="C468" s="6" t="s">
         <v>119</v>
@@ -6937,10 +7036,10 @@
     </row>
     <row r="469" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="7" t="s">
-        <v>470</v>
+        <v>503</v>
       </c>
       <c r="B469" s="8" t="s">
-        <v>529</v>
+        <v>562</v>
       </c>
       <c r="C469" s="6" t="s">
         <v>119</v>
@@ -6959,10 +7058,10 @@
     </row>
     <row r="472" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="7" t="s">
-        <v>530</v>
+        <v>563</v>
       </c>
       <c r="B472" s="8" t="s">
-        <v>531</v>
+        <v>564</v>
       </c>
       <c r="C472" s="6" t="s">
         <v>119</v>
@@ -6970,10 +7069,10 @@
     </row>
     <row r="473" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="7" t="s">
-        <v>530</v>
+        <v>563</v>
       </c>
       <c r="B473" s="8" t="s">
-        <v>532</v>
+        <v>565</v>
       </c>
       <c r="C473" s="6" t="s">
         <v>119</v>
@@ -6981,10 +7080,10 @@
     </row>
     <row r="474" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="7" t="s">
-        <v>530</v>
+        <v>563</v>
       </c>
       <c r="B474" s="8" t="s">
-        <v>533</v>
+        <v>566</v>
       </c>
       <c r="C474" s="6" t="s">
         <v>119</v>
@@ -6992,10 +7091,10 @@
     </row>
     <row r="475" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="7" t="s">
-        <v>530</v>
+        <v>563</v>
       </c>
       <c r="B475" s="8" t="s">
-        <v>534</v>
+        <v>567</v>
       </c>
       <c r="C475" s="6" t="s">
         <v>119</v>
@@ -7003,10 +7102,10 @@
     </row>
     <row r="476" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="7" t="s">
-        <v>530</v>
+        <v>563</v>
       </c>
       <c r="B476" s="8" t="s">
-        <v>535</v>
+        <v>568</v>
       </c>
       <c r="C476" s="6" t="s">
         <v>119</v>
@@ -7014,10 +7113,10 @@
     </row>
     <row r="477" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="7" t="s">
-        <v>530</v>
+        <v>563</v>
       </c>
       <c r="B477" s="8" t="s">
-        <v>536</v>
+        <v>569</v>
       </c>
       <c r="C477" s="6" t="s">
         <v>119</v>
@@ -7025,10 +7124,10 @@
     </row>
     <row r="478" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="7" t="s">
-        <v>530</v>
+        <v>563</v>
       </c>
       <c r="B478" s="8" t="s">
-        <v>537</v>
+        <v>570</v>
       </c>
       <c r="C478" s="6" t="s">
         <v>119</v>
@@ -7036,10 +7135,10 @@
     </row>
     <row r="479" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="7" t="s">
-        <v>530</v>
+        <v>563</v>
       </c>
       <c r="B479" s="8" t="s">
-        <v>538</v>
+        <v>571</v>
       </c>
       <c r="C479" s="6" t="s">
         <v>119</v>
@@ -7047,10 +7146,10 @@
     </row>
     <row r="480" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="7" t="s">
-        <v>530</v>
+        <v>563</v>
       </c>
       <c r="B480" s="8" t="s">
-        <v>539</v>
+        <v>572</v>
       </c>
       <c r="C480" s="6" t="s">
         <v>119</v>
@@ -7058,10 +7157,10 @@
     </row>
     <row r="481" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="7" t="s">
-        <v>530</v>
+        <v>563</v>
       </c>
       <c r="B481" s="8" t="s">
-        <v>540</v>
+        <v>573</v>
       </c>
       <c r="C481" s="6" t="s">
         <v>119</v>

</xml_diff>

<commit_message>
Trie added, optimized string 36
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="580">
   <si>
     <t xml:space="preserve">YES(Iterative &amp; recursive)</t>
   </si>
@@ -1549,16 +1549,34 @@
     <t xml:space="preserve">Construct a trie from scratch</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(insertion,searching,deleting)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Find shortest unique prefix for every word in a given list</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(frequency)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Word Break Problem | (Trie solution)</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(trie+memoization)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES(sort &amp; insert into trie store word in leaf vector)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Implement a Phone Directory</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(DFS)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Print unique rows in a given boolean matrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES(check while insertion)</t>
   </si>
   <si>
     <t xml:space="preserve">Dynamic Programming</t>
@@ -2055,8 +2073,8 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A371" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C400" activeCellId="0" sqref="C400"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A393" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C408" activeCellId="0" sqref="C408"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6308,15 +6326,15 @@
       <c r="B401" s="10"/>
       <c r="C401" s="6"/>
     </row>
-    <row r="402" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="402" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="7" t="s">
         <v>497</v>
       </c>
       <c r="B402" s="8" t="s">
         <v>498</v>
       </c>
-      <c r="C402" s="6" t="s">
-        <v>119</v>
+      <c r="C402" s="9" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6324,10 +6342,10 @@
         <v>497</v>
       </c>
       <c r="B403" s="8" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="C403" s="6" t="s">
-        <v>119</v>
+        <v>501</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6335,10 +6353,10 @@
         <v>497</v>
       </c>
       <c r="B404" s="8" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="C404" s="6" t="s">
-        <v>119</v>
+        <v>503</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6349,18 +6367,18 @@
         <v>122</v>
       </c>
       <c r="C405" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="406" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="406" customFormat="false" ht="19.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="7" t="s">
         <v>497</v>
       </c>
       <c r="B406" s="8" t="s">
-        <v>501</v>
-      </c>
-      <c r="C406" s="6" t="s">
-        <v>119</v>
+        <v>505</v>
+      </c>
+      <c r="C406" s="9" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6368,10 +6386,10 @@
         <v>497</v>
       </c>
       <c r="B407" s="8" t="s">
-        <v>502</v>
+        <v>507</v>
       </c>
       <c r="C407" s="6" t="s">
-        <v>119</v>
+        <v>508</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6387,10 +6405,10 @@
     </row>
     <row r="410" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B410" s="8" t="s">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c r="C410" s="6" t="s">
         <v>119</v>
@@ -6398,10 +6416,10 @@
     </row>
     <row r="411" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B411" s="8" t="s">
-        <v>505</v>
+        <v>511</v>
       </c>
       <c r="C411" s="6" t="s">
         <v>119</v>
@@ -6409,10 +6427,10 @@
     </row>
     <row r="412" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B412" s="8" t="s">
-        <v>506</v>
+        <v>512</v>
       </c>
       <c r="C412" s="6" t="s">
         <v>119</v>
@@ -6420,10 +6438,10 @@
     </row>
     <row r="413" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B413" s="8" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
       <c r="C413" s="6" t="s">
         <v>119</v>
@@ -6431,10 +6449,10 @@
     </row>
     <row r="414" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B414" s="8" t="s">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="C414" s="6" t="s">
         <v>119</v>
@@ -6442,10 +6460,10 @@
     </row>
     <row r="415" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B415" s="8" t="s">
-        <v>509</v>
+        <v>515</v>
       </c>
       <c r="C415" s="6" t="s">
         <v>119</v>
@@ -6453,10 +6471,10 @@
     </row>
     <row r="416" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B416" s="8" t="s">
-        <v>510</v>
+        <v>516</v>
       </c>
       <c r="C416" s="6" t="s">
         <v>119</v>
@@ -6464,7 +6482,7 @@
     </row>
     <row r="417" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B417" s="8" t="s">
         <v>341</v>
@@ -6475,10 +6493,10 @@
     </row>
     <row r="418" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B418" s="8" t="s">
-        <v>511</v>
+        <v>517</v>
       </c>
       <c r="C418" s="6" t="s">
         <v>119</v>
@@ -6486,10 +6504,10 @@
     </row>
     <row r="419" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B419" s="8" t="s">
-        <v>512</v>
+        <v>518</v>
       </c>
       <c r="C419" s="6" t="s">
         <v>119</v>
@@ -6497,10 +6515,10 @@
     </row>
     <row r="420" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B420" s="8" t="s">
-        <v>513</v>
+        <v>519</v>
       </c>
       <c r="C420" s="6" t="s">
         <v>119</v>
@@ -6508,10 +6526,10 @@
     </row>
     <row r="421" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B421" s="8" t="s">
-        <v>514</v>
+        <v>520</v>
       </c>
       <c r="C421" s="6" t="s">
         <v>119</v>
@@ -6519,10 +6537,10 @@
     </row>
     <row r="422" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B422" s="8" t="s">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="C422" s="6" t="s">
         <v>119</v>
@@ -6530,10 +6548,10 @@
     </row>
     <row r="423" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B423" s="8" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="C423" s="6" t="s">
         <v>119</v>
@@ -6541,10 +6559,10 @@
     </row>
     <row r="424" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B424" s="8" t="s">
-        <v>517</v>
+        <v>523</v>
       </c>
       <c r="C424" s="6" t="s">
         <v>119</v>
@@ -6552,10 +6570,10 @@
     </row>
     <row r="425" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B425" s="8" t="s">
-        <v>518</v>
+        <v>524</v>
       </c>
       <c r="C425" s="6" t="s">
         <v>119</v>
@@ -6563,10 +6581,10 @@
     </row>
     <row r="426" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B426" s="8" t="s">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="C426" s="6" t="s">
         <v>119</v>
@@ -6574,10 +6592,10 @@
     </row>
     <row r="427" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B427" s="8" t="s">
-        <v>520</v>
+        <v>526</v>
       </c>
       <c r="C427" s="6" t="s">
         <v>119</v>
@@ -6585,10 +6603,10 @@
     </row>
     <row r="428" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B428" s="8" t="s">
-        <v>521</v>
+        <v>527</v>
       </c>
       <c r="C428" s="6" t="s">
         <v>119</v>
@@ -6596,10 +6614,10 @@
     </row>
     <row r="429" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B429" s="8" t="s">
-        <v>522</v>
+        <v>528</v>
       </c>
       <c r="C429" s="6" t="s">
         <v>119</v>
@@ -6607,10 +6625,10 @@
     </row>
     <row r="430" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B430" s="8" t="s">
-        <v>523</v>
+        <v>529</v>
       </c>
       <c r="C430" s="6" t="s">
         <v>119</v>
@@ -6618,10 +6636,10 @@
     </row>
     <row r="431" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B431" s="8" t="s">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="C431" s="6" t="s">
         <v>119</v>
@@ -6629,10 +6647,10 @@
     </row>
     <row r="432" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B432" s="8" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="C432" s="6" t="s">
         <v>119</v>
@@ -6640,10 +6658,10 @@
     </row>
     <row r="433" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B433" s="8" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="C433" s="6" t="s">
         <v>119</v>
@@ -6651,10 +6669,10 @@
     </row>
     <row r="434" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B434" s="8" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="C434" s="6" t="s">
         <v>119</v>
@@ -6662,10 +6680,10 @@
     </row>
     <row r="435" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B435" s="8" t="s">
-        <v>528</v>
+        <v>534</v>
       </c>
       <c r="C435" s="6" t="s">
         <v>119</v>
@@ -6673,10 +6691,10 @@
     </row>
     <row r="436" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B436" s="8" t="s">
-        <v>529</v>
+        <v>535</v>
       </c>
       <c r="C436" s="6" t="s">
         <v>119</v>
@@ -6684,10 +6702,10 @@
     </row>
     <row r="437" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B437" s="8" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="C437" s="6" t="s">
         <v>119</v>
@@ -6695,10 +6713,10 @@
     </row>
     <row r="438" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B438" s="8" t="s">
-        <v>531</v>
+        <v>537</v>
       </c>
       <c r="C438" s="6" t="s">
         <v>119</v>
@@ -6706,10 +6724,10 @@
     </row>
     <row r="439" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B439" s="8" t="s">
-        <v>532</v>
+        <v>538</v>
       </c>
       <c r="C439" s="6" t="s">
         <v>119</v>
@@ -6717,10 +6735,10 @@
     </row>
     <row r="440" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B440" s="8" t="s">
-        <v>533</v>
+        <v>539</v>
       </c>
       <c r="C440" s="6" t="s">
         <v>119</v>
@@ -6728,10 +6746,10 @@
     </row>
     <row r="441" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B441" s="8" t="s">
-        <v>534</v>
+        <v>540</v>
       </c>
       <c r="C441" s="6" t="s">
         <v>119</v>
@@ -6739,10 +6757,10 @@
     </row>
     <row r="442" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B442" s="8" t="s">
-        <v>535</v>
+        <v>541</v>
       </c>
       <c r="C442" s="6" t="s">
         <v>119</v>
@@ -6750,10 +6768,10 @@
     </row>
     <row r="443" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B443" s="8" t="s">
-        <v>536</v>
+        <v>542</v>
       </c>
       <c r="C443" s="6" t="s">
         <v>119</v>
@@ -6761,10 +6779,10 @@
     </row>
     <row r="444" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B444" s="8" t="s">
-        <v>537</v>
+        <v>543</v>
       </c>
       <c r="C444" s="6" t="s">
         <v>119</v>
@@ -6772,10 +6790,10 @@
     </row>
     <row r="445" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B445" s="8" t="s">
-        <v>538</v>
+        <v>544</v>
       </c>
       <c r="C445" s="6" t="s">
         <v>119</v>
@@ -6783,10 +6801,10 @@
     </row>
     <row r="446" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B446" s="8" t="s">
-        <v>539</v>
+        <v>545</v>
       </c>
       <c r="C446" s="6" t="s">
         <v>119</v>
@@ -6794,10 +6812,10 @@
     </row>
     <row r="447" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B447" s="8" t="s">
-        <v>540</v>
+        <v>546</v>
       </c>
       <c r="C447" s="6" t="s">
         <v>119</v>
@@ -6805,10 +6823,10 @@
     </row>
     <row r="448" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B448" s="8" t="s">
-        <v>541</v>
+        <v>547</v>
       </c>
       <c r="C448" s="6" t="s">
         <v>119</v>
@@ -6816,10 +6834,10 @@
     </row>
     <row r="449" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B449" s="8" t="s">
-        <v>542</v>
+        <v>548</v>
       </c>
       <c r="C449" s="6" t="s">
         <v>119</v>
@@ -6827,10 +6845,10 @@
     </row>
     <row r="450" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B450" s="8" t="s">
-        <v>543</v>
+        <v>549</v>
       </c>
       <c r="C450" s="6" t="s">
         <v>119</v>
@@ -6838,10 +6856,10 @@
     </row>
     <row r="451" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B451" s="8" t="s">
-        <v>544</v>
+        <v>550</v>
       </c>
       <c r="C451" s="6" t="s">
         <v>119</v>
@@ -6849,10 +6867,10 @@
     </row>
     <row r="452" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B452" s="8" t="s">
-        <v>545</v>
+        <v>551</v>
       </c>
       <c r="C452" s="6" t="s">
         <v>119</v>
@@ -6860,10 +6878,10 @@
     </row>
     <row r="453" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B453" s="8" t="s">
-        <v>546</v>
+        <v>552</v>
       </c>
       <c r="C453" s="6" t="s">
         <v>119</v>
@@ -6871,10 +6889,10 @@
     </row>
     <row r="454" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B454" s="8" t="s">
-        <v>547</v>
+        <v>553</v>
       </c>
       <c r="C454" s="6" t="s">
         <v>119</v>
@@ -6882,10 +6900,10 @@
     </row>
     <row r="455" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B455" s="8" t="s">
-        <v>548</v>
+        <v>554</v>
       </c>
       <c r="C455" s="6" t="s">
         <v>119</v>
@@ -6893,10 +6911,10 @@
     </row>
     <row r="456" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B456" s="8" t="s">
-        <v>549</v>
+        <v>555</v>
       </c>
       <c r="C456" s="6" t="s">
         <v>119</v>
@@ -6904,10 +6922,10 @@
     </row>
     <row r="457" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B457" s="8" t="s">
-        <v>550</v>
+        <v>556</v>
       </c>
       <c r="C457" s="6" t="s">
         <v>119</v>
@@ -6915,10 +6933,10 @@
     </row>
     <row r="458" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B458" s="8" t="s">
-        <v>551</v>
+        <v>557</v>
       </c>
       <c r="C458" s="6" t="s">
         <v>119</v>
@@ -6926,10 +6944,10 @@
     </row>
     <row r="459" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B459" s="8" t="s">
-        <v>552</v>
+        <v>558</v>
       </c>
       <c r="C459" s="6" t="s">
         <v>119</v>
@@ -6937,10 +6955,10 @@
     </row>
     <row r="460" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B460" s="8" t="s">
-        <v>553</v>
+        <v>559</v>
       </c>
       <c r="C460" s="6" t="s">
         <v>119</v>
@@ -6948,10 +6966,10 @@
     </row>
     <row r="461" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B461" s="8" t="s">
-        <v>554</v>
+        <v>560</v>
       </c>
       <c r="C461" s="6" t="s">
         <v>119</v>
@@ -6959,10 +6977,10 @@
     </row>
     <row r="462" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B462" s="8" t="s">
-        <v>555</v>
+        <v>561</v>
       </c>
       <c r="C462" s="6" t="s">
         <v>119</v>
@@ -6970,10 +6988,10 @@
     </row>
     <row r="463" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B463" s="8" t="s">
-        <v>556</v>
+        <v>562</v>
       </c>
       <c r="C463" s="6" t="s">
         <v>119</v>
@@ -6981,10 +6999,10 @@
     </row>
     <row r="464" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B464" s="8" t="s">
-        <v>557</v>
+        <v>563</v>
       </c>
       <c r="C464" s="6" t="s">
         <v>119</v>
@@ -6992,10 +7010,10 @@
     </row>
     <row r="465" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B465" s="8" t="s">
-        <v>558</v>
+        <v>564</v>
       </c>
       <c r="C465" s="6" t="s">
         <v>119</v>
@@ -7003,10 +7021,10 @@
     </row>
     <row r="466" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B466" s="8" t="s">
-        <v>559</v>
+        <v>565</v>
       </c>
       <c r="C466" s="6" t="s">
         <v>119</v>
@@ -7014,10 +7032,10 @@
     </row>
     <row r="467" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B467" s="8" t="s">
-        <v>560</v>
+        <v>566</v>
       </c>
       <c r="C467" s="6" t="s">
         <v>119</v>
@@ -7025,10 +7043,10 @@
     </row>
     <row r="468" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B468" s="8" t="s">
-        <v>561</v>
+        <v>567</v>
       </c>
       <c r="C468" s="6" t="s">
         <v>119</v>
@@ -7036,10 +7054,10 @@
     </row>
     <row r="469" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="7" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="B469" s="8" t="s">
-        <v>562</v>
+        <v>568</v>
       </c>
       <c r="C469" s="6" t="s">
         <v>119</v>
@@ -7058,10 +7076,10 @@
     </row>
     <row r="472" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="7" t="s">
-        <v>563</v>
+        <v>569</v>
       </c>
       <c r="B472" s="8" t="s">
-        <v>564</v>
+        <v>570</v>
       </c>
       <c r="C472" s="6" t="s">
         <v>119</v>
@@ -7069,10 +7087,10 @@
     </row>
     <row r="473" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="7" t="s">
-        <v>563</v>
+        <v>569</v>
       </c>
       <c r="B473" s="8" t="s">
-        <v>565</v>
+        <v>571</v>
       </c>
       <c r="C473" s="6" t="s">
         <v>119</v>
@@ -7080,10 +7098,10 @@
     </row>
     <row r="474" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="7" t="s">
-        <v>563</v>
+        <v>569</v>
       </c>
       <c r="B474" s="8" t="s">
-        <v>566</v>
+        <v>572</v>
       </c>
       <c r="C474" s="6" t="s">
         <v>119</v>
@@ -7091,10 +7109,10 @@
     </row>
     <row r="475" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="7" t="s">
-        <v>563</v>
+        <v>569</v>
       </c>
       <c r="B475" s="8" t="s">
-        <v>567</v>
+        <v>573</v>
       </c>
       <c r="C475" s="6" t="s">
         <v>119</v>
@@ -7102,10 +7120,10 @@
     </row>
     <row r="476" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="7" t="s">
-        <v>563</v>
+        <v>569</v>
       </c>
       <c r="B476" s="8" t="s">
-        <v>568</v>
+        <v>574</v>
       </c>
       <c r="C476" s="6" t="s">
         <v>119</v>
@@ -7113,10 +7131,10 @@
     </row>
     <row r="477" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="7" t="s">
-        <v>563</v>
+        <v>569</v>
       </c>
       <c r="B477" s="8" t="s">
-        <v>569</v>
+        <v>575</v>
       </c>
       <c r="C477" s="6" t="s">
         <v>119</v>
@@ -7124,10 +7142,10 @@
     </row>
     <row r="478" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="7" t="s">
-        <v>563</v>
+        <v>569</v>
       </c>
       <c r="B478" s="8" t="s">
-        <v>570</v>
+        <v>576</v>
       </c>
       <c r="C478" s="6" t="s">
         <v>119</v>
@@ -7135,10 +7153,10 @@
     </row>
     <row r="479" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="7" t="s">
-        <v>563</v>
+        <v>569</v>
       </c>
       <c r="B479" s="8" t="s">
-        <v>571</v>
+        <v>577</v>
       </c>
       <c r="C479" s="6" t="s">
         <v>119</v>
@@ -7146,10 +7164,10 @@
     </row>
     <row r="480" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="7" t="s">
-        <v>563</v>
+        <v>569</v>
       </c>
       <c r="B480" s="8" t="s">
-        <v>572</v>
+        <v>578</v>
       </c>
       <c r="C480" s="6" t="s">
         <v>119</v>
@@ -7157,10 +7175,10 @@
     </row>
     <row r="481" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="7" t="s">
-        <v>563</v>
+        <v>569</v>
       </c>
       <c r="B481" s="8" t="s">
-        <v>573</v>
+        <v>579</v>
       </c>
       <c r="C481" s="6" t="s">
         <v>119</v>

</xml_diff>

<commit_message>
Stacks & Queues added, LinkedList 36 explanation revised
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="651">
   <si>
     <t xml:space="preserve">YES(Iterative &amp; recursive)</t>
   </si>
@@ -1147,12 +1147,21 @@
     <t xml:space="preserve">Implement 2 stack in an array</t>
   </si>
   <si>
+    <t xml:space="preserve">y(start from both ends)</t>
+  </si>
+  <si>
     <t xml:space="preserve">find the middle element of a stack</t>
   </si>
   <si>
+    <t xml:space="preserve">y(doubly linked list)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Implement "N" stacks in an Array</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(using next and top arrays)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Check the expression has valid or Balanced parenthesis or not.</t>
   </si>
   <si>
@@ -1162,24 +1171,45 @@
     <t xml:space="preserve">Design a Stack that supports getMin() in O(1) time and O(1) extra space.</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(diff=2e-min, e=2diff-min)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Find the next Greater element</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(stack to maintain increasing order from last)</t>
+  </si>
+  <si>
     <t xml:space="preserve">The celebrity Problem</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(elimination of all person until one potential)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Arithmetic Expression evaluation</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(convert to postfix then evaluate)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Evaluation of Postfix expression</t>
   </si>
   <si>
+    <t xml:space="preserve">y(see above)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Implement a method to insert an element at its bottom without using any other data structure.</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(recursion stack)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reverse a stack using recursion</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(as using above function)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sort a Stack using recursion</t>
   </si>
   <si>
@@ -1189,69 +1219,120 @@
     <t xml:space="preserve">Largest rectangular Area in Histogram</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(use concept of nxt grtr element, see 3 method)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Length of the Longest Valid Substring</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(see strategy of using stack)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Expression contains redundant bracket or not</t>
   </si>
   <si>
+    <t xml:space="preserve">y(true when top is ‘(‘ when ‘)’ is encountered)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Implement Stack using Queue</t>
   </si>
   <si>
     <t xml:space="preserve">Implement Stack using Deque</t>
   </si>
   <si>
+    <t xml:space="preserve">y(if interested see inheritance used when not using stl)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Stack Permutations (Check if an array is stack permutation of other)</t>
   </si>
   <si>
     <t xml:space="preserve">Implement Queue using Stack  </t>
   </si>
   <si>
+    <t xml:space="preserve">y(same as stack using 2 queues)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Implement "n" queue in an array</t>
   </si>
   <si>
+    <t xml:space="preserve">y(similar to n stack in single array)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Implement a Circular queue</t>
   </si>
   <si>
+    <t xml:space="preserve">y(go through once)</t>
+  </si>
+  <si>
     <t xml:space="preserve">LRU Cache Implementationa</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(Doubly linked list and hashmap)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reverse a Queue using recursion</t>
   </si>
   <si>
     <t xml:space="preserve">Reverse the first “K” elements of a queue</t>
   </si>
   <si>
+    <t xml:space="preserve">y(stack stores first k,enqueue and arrange rest)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Interleave the first half of the queue with second half</t>
   </si>
   <si>
+    <t xml:space="preserve">y(see 5 steps)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Find the first circular tour that visits all Petrol Pumps</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(see concept if forgotten)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Minimum time required to rot all oranges</t>
   </si>
   <si>
+    <t xml:space="preserve">YES(BFS)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Distance of nearest cell having 1 in a binary matrix</t>
   </si>
   <si>
+    <t xml:space="preserve">y(BFS)</t>
+  </si>
+  <si>
     <t xml:space="preserve">First negative integer in every window of size “k”</t>
   </si>
   <si>
+    <t xml:space="preserve">y(sliding window using dequeue)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Check if all levels of two trees are anagrams or not.</t>
   </si>
   <si>
+    <t xml:space="preserve">y(level order then sort and check anagram each lvl)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sum of minimum and maximum elements of all subarrays of size “k”.</t>
   </si>
   <si>
     <t xml:space="preserve">Minimum sum of squares of character counts in a given string after removing “k” characters.</t>
   </si>
   <si>
+    <t xml:space="preserve">y(priority queue and frequency hashmap)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Queue based approach or first non-repeating character in a stream.</t>
   </si>
   <si>
     <t xml:space="preserve">Next Smaller Element</t>
   </si>
   <si>
+    <t xml:space="preserve">y(similar as next greater element)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Heap</t>
   </si>
   <si>
@@ -1390,9 +1471,6 @@
     <t xml:space="preserve">word Ladder </t>
   </si>
   <si>
-    <t xml:space="preserve">YES(BFS)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dijkstra algo</t>
   </si>
   <si>
@@ -1457,9 +1535,6 @@
   </si>
   <si>
     <t xml:space="preserve">Snake and Ladders Problem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y(BFS)</t>
   </si>
   <si>
     <t xml:space="preserve">Find bridge in a graph</t>
@@ -2211,11 +2286,11 @@
   </sheetPr>
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A406" colorId="64" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C406" activeCellId="0" sqref="C406"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A298" colorId="64" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C298" activeCellId="0" sqref="C298"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="126.67"/>
@@ -5339,7 +5414,7 @@
         <v>362</v>
       </c>
       <c r="C296" s="6" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5350,7 +5425,7 @@
         <v>363</v>
       </c>
       <c r="C297" s="6" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5361,7 +5436,7 @@
         <v>364</v>
       </c>
       <c r="C298" s="6" t="s">
-        <v>120</v>
+        <v>365</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5369,21 +5444,21 @@
         <v>361</v>
       </c>
       <c r="B299" s="8" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C299" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="300" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="300" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="7" t="s">
         <v>361</v>
       </c>
       <c r="B300" s="8" t="s">
-        <v>366</v>
-      </c>
-      <c r="C300" s="6" t="s">
-        <v>120</v>
+        <v>368</v>
+      </c>
+      <c r="C300" s="9" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5391,10 +5466,10 @@
         <v>361</v>
       </c>
       <c r="B301" s="8" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="C301" s="6" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5402,43 +5477,43 @@
         <v>361</v>
       </c>
       <c r="B302" s="8" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C302" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="303" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="303" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="7" t="s">
         <v>361</v>
       </c>
       <c r="B303" s="8" t="s">
-        <v>369</v>
-      </c>
-      <c r="C303" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="304" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>372</v>
+      </c>
+      <c r="C303" s="9" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="304" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="7" t="s">
         <v>361</v>
       </c>
       <c r="B304" s="8" t="s">
-        <v>370</v>
-      </c>
-      <c r="C304" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="305" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>374</v>
+      </c>
+      <c r="C304" s="9" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="305" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="7" t="s">
         <v>361</v>
       </c>
       <c r="B305" s="8" t="s">
-        <v>371</v>
-      </c>
-      <c r="C305" s="6" t="s">
-        <v>120</v>
+        <v>376</v>
+      </c>
+      <c r="C305" s="9" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5446,10 +5521,10 @@
         <v>361</v>
       </c>
       <c r="B306" s="8" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="C306" s="6" t="s">
-        <v>120</v>
+        <v>379</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5457,21 +5532,21 @@
         <v>361</v>
       </c>
       <c r="B307" s="8" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="C307" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="308" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="308" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="7" t="s">
         <v>361</v>
       </c>
       <c r="B308" s="8" t="s">
-        <v>374</v>
-      </c>
-      <c r="C308" s="6" t="s">
-        <v>120</v>
+        <v>382</v>
+      </c>
+      <c r="C308" s="9" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5479,21 +5554,21 @@
         <v>361</v>
       </c>
       <c r="B309" s="12" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
       <c r="C309" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="310" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="310" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="7" t="s">
         <v>361</v>
       </c>
       <c r="B310" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="C310" s="6" t="s">
-        <v>120</v>
+        <v>386</v>
+      </c>
+      <c r="C310" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5501,32 +5576,32 @@
         <v>361</v>
       </c>
       <c r="B311" s="8" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="C311" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="312" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="312" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="7" t="s">
         <v>361</v>
       </c>
       <c r="B312" s="8" t="s">
-        <v>378</v>
-      </c>
-      <c r="C312" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="313" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>388</v>
+      </c>
+      <c r="C312" s="9" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="313" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="7" t="s">
         <v>361</v>
       </c>
       <c r="B313" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="C313" s="6" t="s">
-        <v>120</v>
+        <v>390</v>
+      </c>
+      <c r="C313" s="9" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5534,21 +5609,21 @@
         <v>361</v>
       </c>
       <c r="B314" s="8" t="s">
-        <v>380</v>
+        <v>392</v>
       </c>
       <c r="C314" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="315" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="315" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="7" t="s">
         <v>361</v>
       </c>
       <c r="B315" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="C315" s="6" t="s">
-        <v>120</v>
+        <v>394</v>
+      </c>
+      <c r="C315" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5556,21 +5631,21 @@
         <v>361</v>
       </c>
       <c r="B316" s="8" t="s">
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="C316" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="317" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="317" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="7" t="s">
         <v>361</v>
       </c>
       <c r="B317" s="8" t="s">
-        <v>383</v>
-      </c>
-      <c r="C317" s="6" t="s">
-        <v>120</v>
+        <v>397</v>
+      </c>
+      <c r="C317" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5578,10 +5653,10 @@
         <v>361</v>
       </c>
       <c r="B318" s="8" t="s">
-        <v>384</v>
+        <v>398</v>
       </c>
       <c r="C318" s="6" t="s">
-        <v>120</v>
+        <v>399</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5589,10 +5664,10 @@
         <v>361</v>
       </c>
       <c r="B319" s="8" t="s">
-        <v>385</v>
+        <v>400</v>
       </c>
       <c r="C319" s="6" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5600,10 +5675,10 @@
         <v>361</v>
       </c>
       <c r="B320" s="8" t="s">
-        <v>386</v>
+        <v>402</v>
       </c>
       <c r="C320" s="6" t="s">
-        <v>120</v>
+        <v>403</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5611,10 +5686,10 @@
         <v>361</v>
       </c>
       <c r="B321" s="8" t="s">
-        <v>387</v>
+        <v>404</v>
       </c>
       <c r="C321" s="6" t="s">
-        <v>120</v>
+        <v>405</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5622,10 +5697,10 @@
         <v>361</v>
       </c>
       <c r="B322" s="8" t="s">
-        <v>388</v>
+        <v>406</v>
       </c>
       <c r="C322" s="6" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5633,10 +5708,10 @@
         <v>361</v>
       </c>
       <c r="B323" s="8" t="s">
-        <v>389</v>
+        <v>407</v>
       </c>
       <c r="C323" s="6" t="s">
-        <v>120</v>
+        <v>408</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5644,32 +5719,32 @@
         <v>361</v>
       </c>
       <c r="B324" s="8" t="s">
-        <v>390</v>
+        <v>409</v>
       </c>
       <c r="C324" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="325" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="325" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="7" t="s">
         <v>361</v>
       </c>
       <c r="B325" s="8" t="s">
-        <v>391</v>
-      </c>
-      <c r="C325" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="326" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>411</v>
+      </c>
+      <c r="C325" s="9" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="326" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="7" t="s">
         <v>361</v>
       </c>
       <c r="B326" s="8" t="s">
-        <v>392</v>
+        <v>413</v>
       </c>
       <c r="C326" s="6" t="s">
-        <v>120</v>
+        <v>414</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5677,10 +5752,10 @@
         <v>361</v>
       </c>
       <c r="B327" s="8" t="s">
-        <v>393</v>
+        <v>415</v>
       </c>
       <c r="C327" s="6" t="s">
-        <v>120</v>
+        <v>416</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5688,10 +5763,10 @@
         <v>361</v>
       </c>
       <c r="B328" s="8" t="s">
-        <v>394</v>
+        <v>417</v>
       </c>
       <c r="C328" s="6" t="s">
-        <v>120</v>
+        <v>418</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5699,10 +5774,10 @@
         <v>361</v>
       </c>
       <c r="B329" s="8" t="s">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="C329" s="6" t="s">
-        <v>120</v>
+        <v>420</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5710,10 +5785,10 @@
         <v>361</v>
       </c>
       <c r="B330" s="8" t="s">
-        <v>396</v>
+        <v>421</v>
       </c>
       <c r="C330" s="6" t="s">
-        <v>120</v>
+        <v>418</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5721,10 +5796,10 @@
         <v>361</v>
       </c>
       <c r="B331" s="8" t="s">
-        <v>397</v>
+        <v>422</v>
       </c>
       <c r="C331" s="6" t="s">
-        <v>120</v>
+        <v>423</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5732,10 +5807,10 @@
         <v>361</v>
       </c>
       <c r="B332" s="8" t="s">
-        <v>398</v>
+        <v>424</v>
       </c>
       <c r="C332" s="6" t="s">
-        <v>120</v>
+        <v>10</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5743,10 +5818,10 @@
         <v>361</v>
       </c>
       <c r="B333" s="8" t="s">
-        <v>399</v>
+        <v>425</v>
       </c>
       <c r="C333" s="6" t="s">
-        <v>120</v>
+        <v>426</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5762,10 +5837,10 @@
     </row>
     <row r="336" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="7" t="s">
-        <v>400</v>
+        <v>427</v>
       </c>
       <c r="B336" s="8" t="s">
-        <v>401</v>
+        <v>428</v>
       </c>
       <c r="C336" s="6" t="s">
         <v>10</v>
@@ -5773,21 +5848,21 @@
     </row>
     <row r="337" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="7" t="s">
-        <v>400</v>
+        <v>427</v>
       </c>
       <c r="B337" s="8" t="s">
-        <v>402</v>
+        <v>429</v>
       </c>
       <c r="C337" s="6" t="s">
-        <v>403</v>
+        <v>430</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="7" t="s">
-        <v>400</v>
+        <v>427</v>
       </c>
       <c r="B338" s="8" t="s">
-        <v>404</v>
+        <v>431</v>
       </c>
       <c r="C338" s="6" t="s">
         <v>8</v>
@@ -5795,43 +5870,43 @@
     </row>
     <row r="339" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="7" t="s">
-        <v>400</v>
+        <v>427</v>
       </c>
       <c r="B339" s="8" t="s">
-        <v>405</v>
+        <v>432</v>
       </c>
       <c r="C339" s="6" t="s">
-        <v>406</v>
+        <v>433</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="7" t="s">
-        <v>400</v>
+        <v>427</v>
       </c>
       <c r="B340" s="8" t="s">
-        <v>407</v>
+        <v>434</v>
       </c>
       <c r="C340" s="6" t="s">
-        <v>408</v>
+        <v>435</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="7" t="s">
-        <v>400</v>
+        <v>427</v>
       </c>
       <c r="B341" s="8" t="s">
-        <v>409</v>
+        <v>436</v>
       </c>
       <c r="C341" s="6" t="s">
-        <v>410</v>
+        <v>437</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="7" t="s">
-        <v>400</v>
+        <v>427</v>
       </c>
       <c r="B342" s="8" t="s">
-        <v>411</v>
+        <v>438</v>
       </c>
       <c r="C342" s="6" t="s">
         <v>8</v>
@@ -5839,10 +5914,10 @@
     </row>
     <row r="343" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="7" t="s">
-        <v>400</v>
+        <v>427</v>
       </c>
       <c r="B343" s="8" t="s">
-        <v>412</v>
+        <v>439</v>
       </c>
       <c r="C343" s="9" t="s">
         <v>10</v>
@@ -5850,10 +5925,10 @@
     </row>
     <row r="344" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="7" t="s">
-        <v>400</v>
+        <v>427</v>
       </c>
       <c r="B344" s="12" t="s">
-        <v>413</v>
+        <v>440</v>
       </c>
       <c r="C344" s="9" t="s">
         <v>10</v>
@@ -5861,43 +5936,43 @@
     </row>
     <row r="345" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="7" t="s">
-        <v>400</v>
+        <v>427</v>
       </c>
       <c r="B345" s="8" t="s">
-        <v>414</v>
+        <v>441</v>
       </c>
       <c r="C345" s="6" t="s">
-        <v>415</v>
+        <v>442</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A346" s="7" t="s">
-        <v>400</v>
+        <v>427</v>
       </c>
       <c r="B346" s="8" t="s">
-        <v>416</v>
+        <v>443</v>
       </c>
       <c r="C346" s="6" t="s">
-        <v>417</v>
+        <v>444</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A347" s="7" t="s">
-        <v>400</v>
+        <v>427</v>
       </c>
       <c r="B347" s="8" t="s">
-        <v>418</v>
+        <v>445</v>
       </c>
       <c r="C347" s="9" t="s">
-        <v>419</v>
+        <v>446</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A348" s="7" t="s">
-        <v>400</v>
+        <v>427</v>
       </c>
       <c r="B348" s="8" t="s">
-        <v>420</v>
+        <v>447</v>
       </c>
       <c r="C348" s="6" t="s">
         <v>10</v>
@@ -5905,10 +5980,10 @@
     </row>
     <row r="349" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A349" s="7" t="s">
-        <v>400</v>
+        <v>427</v>
       </c>
       <c r="B349" s="8" t="s">
-        <v>421</v>
+        <v>448</v>
       </c>
       <c r="C349" s="6" t="s">
         <v>8</v>
@@ -5916,21 +5991,21 @@
     </row>
     <row r="350" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A350" s="7" t="s">
-        <v>400</v>
+        <v>427</v>
       </c>
       <c r="B350" s="8" t="s">
-        <v>422</v>
+        <v>449</v>
       </c>
       <c r="C350" s="6" t="s">
-        <v>423</v>
+        <v>450</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A351" s="7" t="s">
-        <v>400</v>
+        <v>427</v>
       </c>
       <c r="B351" s="8" t="s">
-        <v>424</v>
+        <v>451</v>
       </c>
       <c r="C351" s="6" t="s">
         <v>8</v>
@@ -5938,21 +6013,21 @@
     </row>
     <row r="352" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A352" s="7" t="s">
-        <v>400</v>
+        <v>427</v>
       </c>
       <c r="B352" s="8" t="s">
-        <v>425</v>
+        <v>452</v>
       </c>
       <c r="C352" s="6" t="s">
-        <v>426</v>
+        <v>453</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A353" s="7" t="s">
-        <v>400</v>
+        <v>427</v>
       </c>
       <c r="B353" s="8" t="s">
-        <v>427</v>
+        <v>454</v>
       </c>
       <c r="C353" s="6" t="s">
         <v>10</v>
@@ -5971,10 +6046,10 @@
     </row>
     <row r="356" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B356" s="8" t="s">
-        <v>429</v>
+        <v>456</v>
       </c>
       <c r="C356" s="9" t="s">
         <v>10</v>
@@ -5982,10 +6057,10 @@
     </row>
     <row r="357" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B357" s="8" t="s">
-        <v>430</v>
+        <v>457</v>
       </c>
       <c r="C357" s="9" t="s">
         <v>10</v>
@@ -5993,10 +6068,10 @@
     </row>
     <row r="358" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B358" s="8" t="s">
-        <v>431</v>
+        <v>458</v>
       </c>
       <c r="C358" s="9" t="s">
         <v>10</v>
@@ -6004,32 +6079,32 @@
     </row>
     <row r="359" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B359" s="8" t="s">
-        <v>432</v>
+        <v>459</v>
       </c>
       <c r="C359" s="9" t="s">
-        <v>433</v>
+        <v>460</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B360" s="8" t="s">
-        <v>434</v>
+        <v>461</v>
       </c>
       <c r="C360" s="9" t="s">
-        <v>435</v>
+        <v>462</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B361" s="8" t="s">
-        <v>436</v>
+        <v>463</v>
       </c>
       <c r="C361" s="6" t="s">
         <v>265</v>
@@ -6037,65 +6112,65 @@
     </row>
     <row r="362" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B362" s="8" t="s">
-        <v>437</v>
+        <v>464</v>
       </c>
       <c r="C362" s="9" t="s">
-        <v>438</v>
+        <v>465</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B363" s="8" t="s">
-        <v>439</v>
+        <v>466</v>
       </c>
       <c r="C363" s="9" t="s">
-        <v>440</v>
+        <v>467</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B364" s="8" t="s">
-        <v>441</v>
+        <v>468</v>
       </c>
       <c r="C364" s="9" t="s">
-        <v>442</v>
+        <v>469</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B365" s="8" t="s">
-        <v>443</v>
+        <v>470</v>
       </c>
       <c r="C365" s="9" t="s">
-        <v>444</v>
+        <v>471</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B366" s="8" t="s">
-        <v>445</v>
+        <v>472</v>
       </c>
       <c r="C366" s="6" t="s">
-        <v>446</v>
+        <v>414</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B367" s="8" t="s">
-        <v>447</v>
+        <v>473</v>
       </c>
       <c r="C367" s="9" t="s">
         <v>10</v>
@@ -6103,109 +6178,109 @@
     </row>
     <row r="368" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B368" s="8" t="s">
-        <v>448</v>
+        <v>474</v>
       </c>
       <c r="C368" s="6" t="s">
-        <v>449</v>
+        <v>475</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B369" s="8" t="s">
-        <v>450</v>
+        <v>476</v>
       </c>
       <c r="C369" s="6" t="s">
-        <v>449</v>
+        <v>475</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B370" s="8" t="s">
-        <v>451</v>
+        <v>477</v>
       </c>
       <c r="C370" s="6" t="s">
-        <v>449</v>
+        <v>475</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B371" s="8" t="s">
-        <v>452</v>
+        <v>478</v>
       </c>
       <c r="C371" s="9" t="s">
-        <v>453</v>
+        <v>479</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B372" s="8" t="s">
-        <v>454</v>
+        <v>480</v>
       </c>
       <c r="C372" s="9" t="s">
-        <v>455</v>
+        <v>481</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B373" s="8" t="s">
-        <v>456</v>
+        <v>482</v>
       </c>
       <c r="C373" s="9" t="s">
-        <v>457</v>
+        <v>483</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B374" s="8" t="s">
-        <v>458</v>
+        <v>484</v>
       </c>
       <c r="C374" s="9" t="s">
-        <v>459</v>
+        <v>485</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B375" s="8" t="s">
-        <v>460</v>
+        <v>486</v>
       </c>
       <c r="C375" s="9" t="s">
-        <v>461</v>
+        <v>487</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B376" s="8" t="s">
-        <v>462</v>
+        <v>488</v>
       </c>
       <c r="C376" s="9" t="s">
-        <v>457</v>
+        <v>483</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B377" s="8" t="s">
-        <v>463</v>
+        <v>489</v>
       </c>
       <c r="C377" s="9" t="s">
         <v>129</v>
@@ -6213,76 +6288,76 @@
     </row>
     <row r="378" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B378" s="8" t="s">
-        <v>464</v>
+        <v>490</v>
       </c>
       <c r="C378" s="9" t="s">
-        <v>465</v>
+        <v>491</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B379" s="8" t="s">
-        <v>466</v>
+        <v>492</v>
       </c>
       <c r="C379" s="9" t="s">
-        <v>467</v>
+        <v>493</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B380" s="8" t="s">
-        <v>468</v>
+        <v>494</v>
       </c>
       <c r="C380" s="6" t="s">
-        <v>469</v>
+        <v>416</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B381" s="8" t="s">
-        <v>470</v>
+        <v>495</v>
       </c>
       <c r="C381" s="9" t="s">
-        <v>471</v>
+        <v>496</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B382" s="8" t="s">
-        <v>472</v>
+        <v>497</v>
       </c>
       <c r="C382" s="9" t="s">
-        <v>473</v>
+        <v>498</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B383" s="8" t="s">
-        <v>474</v>
+        <v>499</v>
       </c>
       <c r="C383" s="9" t="s">
-        <v>475</v>
+        <v>500</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B384" s="8" t="s">
-        <v>476</v>
+        <v>501</v>
       </c>
       <c r="C384" s="6" t="s">
         <v>8</v>
@@ -6290,65 +6365,65 @@
     </row>
     <row r="385" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B385" s="8" t="s">
-        <v>477</v>
+        <v>502</v>
       </c>
       <c r="C385" s="9" t="s">
-        <v>478</v>
+        <v>503</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B386" s="8" t="s">
-        <v>479</v>
+        <v>504</v>
       </c>
       <c r="C386" s="9" t="s">
-        <v>480</v>
+        <v>505</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B387" s="8" t="s">
-        <v>481</v>
+        <v>506</v>
       </c>
       <c r="C387" s="9" t="s">
-        <v>482</v>
+        <v>507</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B388" s="8" t="s">
-        <v>483</v>
+        <v>508</v>
       </c>
       <c r="C388" s="9" t="s">
-        <v>484</v>
+        <v>509</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B389" s="8" t="s">
-        <v>485</v>
+        <v>510</v>
       </c>
       <c r="C389" s="9" t="s">
-        <v>486</v>
+        <v>511</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B390" s="8" t="s">
-        <v>485</v>
+        <v>510</v>
       </c>
       <c r="C390" s="6" t="s">
         <v>8</v>
@@ -6356,101 +6431,101 @@
     </row>
     <row r="391" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B391" s="8" t="s">
-        <v>487</v>
+        <v>512</v>
       </c>
       <c r="C391" s="9" t="s">
-        <v>488</v>
+        <v>513</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B392" s="8" t="s">
-        <v>489</v>
+        <v>514</v>
       </c>
       <c r="C392" s="6" t="s">
-        <v>490</v>
+        <v>515</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B393" s="8" t="s">
-        <v>491</v>
+        <v>516</v>
       </c>
       <c r="C393" s="9" t="s">
-        <v>492</v>
+        <v>517</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B394" s="8" t="s">
-        <v>493</v>
+        <v>518</v>
       </c>
       <c r="C394" s="9" t="s">
-        <v>494</v>
+        <v>519</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B395" s="8" t="s">
-        <v>495</v>
+        <v>520</v>
       </c>
       <c r="C395" s="9" t="s">
-        <v>496</v>
+        <v>521</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B396" s="8" t="s">
-        <v>497</v>
+        <v>522</v>
       </c>
       <c r="C396" s="11" t="s">
-        <v>498</v>
+        <v>523</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B397" s="8" t="s">
-        <v>499</v>
+        <v>524</v>
       </c>
       <c r="C397" s="9" t="s">
-        <v>500</v>
+        <v>525</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B398" s="8" t="s">
-        <v>501</v>
+        <v>526</v>
       </c>
       <c r="C398" s="9" t="s">
-        <v>502</v>
+        <v>527</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="7" t="s">
-        <v>428</v>
+        <v>455</v>
       </c>
       <c r="B399" s="8" t="s">
-        <v>503</v>
+        <v>528</v>
       </c>
       <c r="C399" s="9" t="s">
-        <v>504</v>
+        <v>529</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6466,68 +6541,68 @@
     </row>
     <row r="402" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="7" t="s">
-        <v>505</v>
+        <v>530</v>
       </c>
       <c r="B402" s="8" t="s">
-        <v>506</v>
+        <v>531</v>
       </c>
       <c r="C402" s="9" t="s">
-        <v>507</v>
+        <v>532</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="7" t="s">
-        <v>505</v>
+        <v>530</v>
       </c>
       <c r="B403" s="8" t="s">
-        <v>508</v>
+        <v>533</v>
       </c>
       <c r="C403" s="6" t="s">
-        <v>509</v>
+        <v>534</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="7" t="s">
-        <v>505</v>
+        <v>530</v>
       </c>
       <c r="B404" s="8" t="s">
-        <v>510</v>
+        <v>535</v>
       </c>
       <c r="C404" s="6" t="s">
-        <v>511</v>
+        <v>536</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="7" t="s">
-        <v>505</v>
+        <v>530</v>
       </c>
       <c r="B405" s="8" t="s">
         <v>123</v>
       </c>
       <c r="C405" s="6" t="s">
-        <v>512</v>
+        <v>537</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="7" t="s">
-        <v>505</v>
+        <v>530</v>
       </c>
       <c r="B406" s="8" t="s">
-        <v>513</v>
+        <v>538</v>
       </c>
       <c r="C406" s="9" t="s">
-        <v>514</v>
+        <v>539</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="7" t="s">
-        <v>505</v>
+        <v>530</v>
       </c>
       <c r="B407" s="8" t="s">
-        <v>515</v>
+        <v>540</v>
       </c>
       <c r="C407" s="6" t="s">
-        <v>516</v>
+        <v>541</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6543,10 +6618,10 @@
     </row>
     <row r="410" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B410" s="8" t="s">
-        <v>518</v>
+        <v>543</v>
       </c>
       <c r="C410" s="6" t="s">
         <v>8</v>
@@ -6554,10 +6629,10 @@
     </row>
     <row r="411" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B411" s="8" t="s">
-        <v>519</v>
+        <v>544</v>
       </c>
       <c r="C411" s="6" t="s">
         <v>8</v>
@@ -6565,54 +6640,54 @@
     </row>
     <row r="412" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B412" s="8" t="s">
-        <v>520</v>
+        <v>545</v>
       </c>
       <c r="C412" s="6" t="s">
-        <v>521</v>
+        <v>546</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B413" s="8" t="s">
-        <v>522</v>
+        <v>547</v>
       </c>
       <c r="C413" s="6" t="s">
-        <v>523</v>
+        <v>548</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B414" s="8" t="s">
-        <v>524</v>
+        <v>549</v>
       </c>
       <c r="C414" s="6" t="s">
-        <v>525</v>
+        <v>550</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B415" s="8" t="s">
-        <v>526</v>
+        <v>551</v>
       </c>
       <c r="C415" s="6" t="s">
-        <v>527</v>
+        <v>552</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B416" s="8" t="s">
-        <v>528</v>
+        <v>553</v>
       </c>
       <c r="C416" s="9" t="s">
         <v>10</v>
@@ -6620,7 +6695,7 @@
     </row>
     <row r="417" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B417" s="8" t="s">
         <v>343</v>
@@ -6631,21 +6706,21 @@
     </row>
     <row r="418" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B418" s="8" t="s">
-        <v>529</v>
+        <v>554</v>
       </c>
       <c r="C418" s="6" t="s">
-        <v>530</v>
+        <v>555</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B419" s="8" t="s">
-        <v>531</v>
+        <v>556</v>
       </c>
       <c r="C419" s="6" t="s">
         <v>8</v>
@@ -6653,10 +6728,10 @@
     </row>
     <row r="420" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B420" s="8" t="s">
-        <v>532</v>
+        <v>557</v>
       </c>
       <c r="C420" s="6" t="s">
         <v>8</v>
@@ -6664,21 +6739,21 @@
     </row>
     <row r="421" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B421" s="8" t="s">
-        <v>533</v>
+        <v>558</v>
       </c>
       <c r="C421" s="6" t="s">
-        <v>534</v>
+        <v>559</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B422" s="8" t="s">
-        <v>535</v>
+        <v>560</v>
       </c>
       <c r="C422" s="6" t="s">
         <v>10</v>
@@ -6686,10 +6761,10 @@
     </row>
     <row r="423" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B423" s="8" t="s">
-        <v>536</v>
+        <v>561</v>
       </c>
       <c r="C423" s="6" t="s">
         <v>8</v>
@@ -6697,10 +6772,10 @@
     </row>
     <row r="424" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B424" s="8" t="s">
-        <v>537</v>
+        <v>562</v>
       </c>
       <c r="C424" s="6" t="s">
         <v>10</v>
@@ -6708,54 +6783,54 @@
     </row>
     <row r="425" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B425" s="8" t="s">
-        <v>538</v>
+        <v>563</v>
       </c>
       <c r="C425" s="9" t="s">
-        <v>539</v>
+        <v>564</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B426" s="8" t="s">
-        <v>540</v>
+        <v>565</v>
       </c>
       <c r="C426" s="6" t="s">
-        <v>541</v>
+        <v>566</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B427" s="8" t="s">
-        <v>542</v>
+        <v>567</v>
       </c>
       <c r="C427" s="6" t="s">
-        <v>543</v>
+        <v>568</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B428" s="8" t="s">
-        <v>544</v>
+        <v>569</v>
       </c>
       <c r="C428" s="9" t="s">
-        <v>545</v>
+        <v>570</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B429" s="8" t="s">
-        <v>546</v>
+        <v>571</v>
       </c>
       <c r="C429" s="9" t="s">
         <v>10</v>
@@ -6763,21 +6838,21 @@
     </row>
     <row r="430" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B430" s="8" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="C430" s="9" t="s">
-        <v>548</v>
+        <v>573</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B431" s="8" t="s">
-        <v>549</v>
+        <v>574</v>
       </c>
       <c r="C431" s="9" t="s">
         <v>10</v>
@@ -6785,10 +6860,10 @@
     </row>
     <row r="432" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B432" s="8" t="s">
-        <v>550</v>
+        <v>575</v>
       </c>
       <c r="C432" s="9" t="s">
         <v>10</v>
@@ -6796,32 +6871,32 @@
     </row>
     <row r="433" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B433" s="8" t="s">
-        <v>551</v>
+        <v>576</v>
       </c>
       <c r="C433" s="6" t="s">
-        <v>552</v>
+        <v>577</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B434" s="8" t="s">
-        <v>553</v>
+        <v>578</v>
       </c>
       <c r="C434" s="9" t="s">
-        <v>554</v>
+        <v>579</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B435" s="8" t="s">
-        <v>555</v>
+        <v>580</v>
       </c>
       <c r="C435" s="6" t="s">
         <v>10</v>
@@ -6829,10 +6904,10 @@
     </row>
     <row r="436" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B436" s="8" t="s">
-        <v>556</v>
+        <v>581</v>
       </c>
       <c r="C436" s="6" t="s">
         <v>8</v>
@@ -6840,10 +6915,10 @@
     </row>
     <row r="437" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B437" s="8" t="s">
-        <v>557</v>
+        <v>582</v>
       </c>
       <c r="C437" s="9" t="s">
         <v>21</v>
@@ -6851,21 +6926,21 @@
     </row>
     <row r="438" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B438" s="8" t="s">
-        <v>558</v>
+        <v>583</v>
       </c>
       <c r="C438" s="9" t="s">
-        <v>559</v>
+        <v>584</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B439" s="8" t="s">
-        <v>560</v>
+        <v>585</v>
       </c>
       <c r="C439" s="6" t="s">
         <v>8</v>
@@ -6873,21 +6948,21 @@
     </row>
     <row r="440" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B440" s="8" t="s">
-        <v>561</v>
+        <v>586</v>
       </c>
       <c r="C440" s="9" t="s">
-        <v>562</v>
+        <v>587</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B441" s="8" t="s">
-        <v>563</v>
+        <v>588</v>
       </c>
       <c r="C441" s="6" t="s">
         <v>8</v>
@@ -6895,21 +6970,21 @@
     </row>
     <row r="442" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B442" s="8" t="s">
-        <v>564</v>
+        <v>589</v>
       </c>
       <c r="C442" s="6" t="s">
-        <v>565</v>
+        <v>590</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B443" s="8" t="s">
-        <v>566</v>
+        <v>591</v>
       </c>
       <c r="C443" s="9" t="s">
         <v>10</v>
@@ -6917,10 +6992,10 @@
     </row>
     <row r="444" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B444" s="8" t="s">
-        <v>567</v>
+        <v>592</v>
       </c>
       <c r="C444" s="9" t="s">
         <v>21</v>
@@ -6928,21 +7003,21 @@
     </row>
     <row r="445" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B445" s="8" t="s">
-        <v>568</v>
+        <v>593</v>
       </c>
       <c r="C445" s="6" t="s">
-        <v>569</v>
+        <v>594</v>
       </c>
     </row>
     <row r="446" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B446" s="8" t="s">
-        <v>570</v>
+        <v>595</v>
       </c>
       <c r="C446" s="6" t="s">
         <v>8</v>
@@ -6950,21 +7025,21 @@
     </row>
     <row r="447" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B447" s="8" t="s">
-        <v>571</v>
+        <v>596</v>
       </c>
       <c r="C447" s="6" t="s">
-        <v>572</v>
+        <v>597</v>
       </c>
     </row>
     <row r="448" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B448" s="8" t="s">
-        <v>573</v>
+        <v>598</v>
       </c>
       <c r="C448" s="9" t="s">
         <v>10</v>
@@ -6972,10 +7047,10 @@
     </row>
     <row r="449" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B449" s="8" t="s">
-        <v>574</v>
+        <v>599</v>
       </c>
       <c r="C449" s="6" t="s">
         <v>8</v>
@@ -6983,10 +7058,10 @@
     </row>
     <row r="450" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B450" s="8" t="s">
-        <v>575</v>
+        <v>600</v>
       </c>
       <c r="C450" s="6" t="s">
         <v>8</v>
@@ -6994,54 +7069,54 @@
     </row>
     <row r="451" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B451" s="8" t="s">
-        <v>576</v>
+        <v>601</v>
       </c>
       <c r="C451" s="9" t="s">
-        <v>577</v>
+        <v>602</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B452" s="8" t="s">
-        <v>578</v>
+        <v>603</v>
       </c>
       <c r="C452" s="6" t="s">
-        <v>579</v>
+        <v>604</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B453" s="8" t="s">
-        <v>580</v>
+        <v>605</v>
       </c>
       <c r="C453" s="9" t="s">
-        <v>581</v>
+        <v>606</v>
       </c>
     </row>
     <row r="454" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B454" s="8" t="s">
-        <v>582</v>
+        <v>607</v>
       </c>
       <c r="C454" s="9" t="s">
-        <v>583</v>
+        <v>608</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B455" s="8" t="s">
-        <v>584</v>
+        <v>609</v>
       </c>
       <c r="C455" s="9" t="s">
         <v>10</v>
@@ -7049,10 +7124,10 @@
     </row>
     <row r="456" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B456" s="8" t="s">
-        <v>585</v>
+        <v>610</v>
       </c>
       <c r="C456" s="9" t="s">
         <v>10</v>
@@ -7060,145 +7135,145 @@
     </row>
     <row r="457" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B457" s="8" t="s">
-        <v>586</v>
+        <v>611</v>
       </c>
       <c r="C457" s="9" t="s">
-        <v>587</v>
+        <v>612</v>
       </c>
     </row>
     <row r="458" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B458" s="8" t="s">
-        <v>588</v>
+        <v>613</v>
       </c>
       <c r="C458" s="9" t="s">
-        <v>589</v>
+        <v>614</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B459" s="8" t="s">
-        <v>590</v>
+        <v>615</v>
       </c>
       <c r="C459" s="9" t="s">
-        <v>591</v>
+        <v>616</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B460" s="8" t="s">
-        <v>592</v>
+        <v>617</v>
       </c>
       <c r="C460" s="9" t="s">
-        <v>593</v>
+        <v>618</v>
       </c>
     </row>
     <row r="461" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B461" s="8" t="s">
-        <v>594</v>
+        <v>619</v>
       </c>
       <c r="C461" s="9" t="s">
-        <v>595</v>
+        <v>620</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B462" s="8" t="s">
-        <v>596</v>
+        <v>621</v>
       </c>
       <c r="C462" s="9" t="s">
-        <v>597</v>
+        <v>622</v>
       </c>
     </row>
     <row r="463" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B463" s="8" t="s">
-        <v>598</v>
+        <v>623</v>
       </c>
       <c r="C463" s="9" t="s">
-        <v>599</v>
+        <v>624</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B464" s="8" t="s">
-        <v>600</v>
+        <v>625</v>
       </c>
       <c r="C464" s="9" t="s">
-        <v>601</v>
+        <v>626</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B465" s="8" t="s">
-        <v>602</v>
+        <v>627</v>
       </c>
       <c r="C465" s="6" t="s">
-        <v>603</v>
+        <v>628</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B466" s="8" t="s">
-        <v>604</v>
+        <v>629</v>
       </c>
       <c r="C466" s="9" t="s">
-        <v>605</v>
+        <v>630</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B467" s="8" t="s">
-        <v>606</v>
+        <v>631</v>
       </c>
       <c r="C467" s="9" t="s">
-        <v>607</v>
+        <v>632</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="22.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B468" s="8" t="s">
-        <v>608</v>
+        <v>633</v>
       </c>
       <c r="C468" s="9" t="s">
-        <v>609</v>
+        <v>634</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="7" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B469" s="8" t="s">
-        <v>610</v>
+        <v>635</v>
       </c>
       <c r="C469" s="6" t="s">
-        <v>548</v>
+        <v>573</v>
       </c>
     </row>
     <row r="470" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7214,10 +7289,10 @@
     </row>
     <row r="472" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="7" t="s">
-        <v>611</v>
+        <v>636</v>
       </c>
       <c r="B472" s="8" t="s">
-        <v>612</v>
+        <v>637</v>
       </c>
       <c r="C472" s="6" t="s">
         <v>8</v>
@@ -7225,21 +7300,21 @@
     </row>
     <row r="473" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="7" t="s">
-        <v>611</v>
+        <v>636</v>
       </c>
       <c r="B473" s="8" t="s">
-        <v>613</v>
+        <v>638</v>
       </c>
       <c r="C473" s="6" t="s">
-        <v>614</v>
+        <v>639</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="7" t="s">
-        <v>611</v>
+        <v>636</v>
       </c>
       <c r="B474" s="8" t="s">
-        <v>615</v>
+        <v>640</v>
       </c>
       <c r="C474" s="6" t="s">
         <v>8</v>
@@ -7247,32 +7322,32 @@
     </row>
     <row r="475" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="7" t="s">
-        <v>611</v>
+        <v>636</v>
       </c>
       <c r="B475" s="8" t="s">
-        <v>616</v>
+        <v>641</v>
       </c>
       <c r="C475" s="9" t="s">
-        <v>617</v>
+        <v>642</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="7" t="s">
-        <v>611</v>
+        <v>636</v>
       </c>
       <c r="B476" s="8" t="s">
-        <v>618</v>
+        <v>643</v>
       </c>
       <c r="C476" s="9" t="s">
-        <v>619</v>
+        <v>644</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="7" t="s">
-        <v>611</v>
+        <v>636</v>
       </c>
       <c r="B477" s="8" t="s">
-        <v>620</v>
+        <v>645</v>
       </c>
       <c r="C477" s="9" t="s">
         <v>10</v>
@@ -7280,21 +7355,21 @@
     </row>
     <row r="478" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="7" t="s">
-        <v>611</v>
+        <v>636</v>
       </c>
       <c r="B478" s="8" t="s">
-        <v>621</v>
+        <v>646</v>
       </c>
       <c r="C478" s="9" t="s">
-        <v>622</v>
+        <v>647</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="7" t="s">
-        <v>611</v>
+        <v>636</v>
       </c>
       <c r="B479" s="8" t="s">
-        <v>623</v>
+        <v>648</v>
       </c>
       <c r="C479" s="9" t="s">
         <v>10</v>
@@ -7302,10 +7377,10 @@
     </row>
     <row r="480" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="7" t="s">
-        <v>611</v>
+        <v>636</v>
       </c>
       <c r="B480" s="8" t="s">
-        <v>624</v>
+        <v>649</v>
       </c>
       <c r="C480" s="9" t="s">
         <v>10</v>
@@ -7313,10 +7388,10 @@
     </row>
     <row r="481" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="7" t="s">
-        <v>611</v>
+        <v>636</v>
       </c>
       <c r="B481" s="8" t="s">
-        <v>625</v>
+        <v>650</v>
       </c>
       <c r="C481" s="9" t="s">
         <v>10</v>

</xml_diff>